<commit_message>
Update logs for next test batch
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -77,12 +77,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>StartDouble3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Reads from :00 to :20, feeds raw samples into the neural network, and then attempts to categorize them into three genres: art, pop, or traditional.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Test Name</t>
   </si>
@@ -124,6 +146,18 @@
   </si>
   <si>
     <t>Random chance</t>
+  </si>
+  <si>
+    <t>SDU3.1</t>
+  </si>
+  <si>
+    <t>StartDouble3</t>
+  </si>
+  <si>
+    <t>SDU3.2</t>
+  </si>
+  <si>
+    <t>SDU3.3</t>
   </si>
 </sst>
 </file>
@@ -461,16 +495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -507,7 +541,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f>1/3</f>
+        <f t="shared" ref="D2:D10" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -526,11 +560,11 @@
         <v>0.76953125</v>
       </c>
       <c r="D3" s="1">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E7" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E10" si="1">C3/D3</f>
         <v>2.30859375</v>
       </c>
     </row>
@@ -545,11 +579,11 @@
         <v>0.76171875</v>
       </c>
       <c r="D4" s="1">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.28515625</v>
       </c>
     </row>
@@ -564,11 +598,11 @@
         <v>0.76171875</v>
       </c>
       <c r="D5" s="1">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.28515625</v>
       </c>
     </row>
@@ -583,11 +617,11 @@
         <v>0.7421875</v>
       </c>
       <c r="D6" s="1">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2265625</v>
       </c>
     </row>
@@ -602,12 +636,60 @@
         <v>0.75390625</v>
       </c>
       <c r="D7" s="1">
-        <f>1/3</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.26171875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final test of this branch
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="7840" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -194,12 +194,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,11 +221,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +579,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,7 +599,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -766,7 +773,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" si="2"/>
-        <v>1.4765625</v>
+        <v>2.265625</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -789,7 +796,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" si="2"/>
-        <v>1.4765625</v>
+        <v>2.265625</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -799,28 +806,31 @@
       <c r="B10" t="s">
         <v>15</v>
       </c>
+      <c r="C10" s="1">
+        <v>0.7890625</v>
+      </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.3671875</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="2"/>
-        <v>1.4765625</v>
+        <v>2.265625</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="3" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Prep for new test
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="7840" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Test Name</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t>Group Change</t>
+  </si>
+  <si>
+    <t>NSP3.1</t>
+  </si>
+  <si>
+    <t>NSP3.2</t>
+  </si>
+  <si>
+    <t>NSP3.3</t>
+  </si>
+  <si>
+    <t>NewShape3</t>
   </si>
 </sst>
 </file>
@@ -232,7 +244,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -576,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +668,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D10" si="0">1/3</f>
+        <f t="shared" ref="D2:D13" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -653,11 +695,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E10" si="1">C3/D3</f>
+        <f t="shared" ref="E3:E13" si="1">C3/D3</f>
         <v>2.30859375</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F10" si="2">AVERAGEIF(B:B,B3,E:E)</f>
+        <f t="shared" ref="F3:F13" si="2">AVERAGEIF(B:B,B3,E:E)</f>
         <v>2.296875</v>
       </c>
     </row>
@@ -822,15 +864,75 @@
         <v>2.265625</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="1" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="2" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Final notes for the day
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -99,12 +99,71 @@
         </r>
       </text>
     </comment>
+    <comment ref="B11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">NewShape3
+Testing the same thing as StartDouble3, but with the initial layer of the NN widened out to 2* size.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">DeeperNN
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Testing the same thing as NewShape3, but with an additional 64-neuron, tanh layer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">MidpointWide
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Testing the same thing as NewShape3, but using the :10-:30 chunk instead of :00-:20
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Test Name</t>
   </si>
@@ -173,6 +232,78 @@
   </si>
   <si>
     <t>NewShape3</t>
+  </si>
+  <si>
+    <t>MidpointWide</t>
+  </si>
+  <si>
+    <t>MDPW.1</t>
+  </si>
+  <si>
+    <t>MDPW.2</t>
+  </si>
+  <si>
+    <t>MDPW.3</t>
+  </si>
+  <si>
+    <t>DNN3.1</t>
+  </si>
+  <si>
+    <t>DNN3.2</t>
+  </si>
+  <si>
+    <t>DNN3.3</t>
+  </si>
+  <si>
+    <t>DeeperNN</t>
+  </si>
+  <si>
+    <t>Logfile</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>09.16.txt</t>
+  </si>
+  <si>
+    <t>09.29.txt</t>
+  </si>
+  <si>
+    <t>09.40.txt</t>
+  </si>
+  <si>
+    <t>09.50.txt</t>
+  </si>
+  <si>
+    <t>09.58.txt</t>
+  </si>
+  <si>
+    <t>10.07.txt</t>
+  </si>
+  <si>
+    <t>11.06.txt</t>
+  </si>
+  <si>
+    <t>11.21.txt</t>
+  </si>
+  <si>
+    <t>13.13.txt</t>
+  </si>
+  <si>
+    <t>15.16.txt</t>
+  </si>
+  <si>
+    <t>15.50.txt</t>
+  </si>
+  <si>
+    <t>15.51.txt</t>
+  </si>
+  <si>
+    <t>16.13.txt</t>
+  </si>
+  <si>
+    <t>16.39.txt</t>
   </si>
 </sst>
 </file>
@@ -233,18 +364,187 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -258,52 +558,6 @@
         </top>
         <bottom style="thin">
           <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
         </bottom>
       </border>
     </dxf>
@@ -690,23 +944,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -725,11 +980,17 @@
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -740,7 +1001,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D13" si="0">1/3</f>
+        <f t="shared" ref="D2:D19" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -751,8 +1012,14 @@
         <f>AVERAGEIF(B:B,B2,E:E)</f>
         <v>2.296875</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -767,15 +1034,21 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E13" si="1">C3/D3</f>
+        <f t="shared" ref="E3:E19" si="1">C3/D3</f>
         <v>2.30859375</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F13" si="2">AVERAGEIF(B:B,B3,E:E)</f>
+        <f t="shared" ref="F3:F19" si="2">AVERAGEIF(B:B,B3,E:E)</f>
         <v>2.296875</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -797,8 +1070,14 @@
         <f t="shared" si="2"/>
         <v>2.296875</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -820,8 +1099,14 @@
         <f t="shared" si="2"/>
         <v>2.2578125</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -843,8 +1128,14 @@
         <f t="shared" si="2"/>
         <v>2.2578125</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -866,8 +1157,14 @@
         <f t="shared" si="2"/>
         <v>2.2578125</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -889,8 +1186,14 @@
         <f t="shared" si="2"/>
         <v>2.265625</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -912,8 +1215,14 @@
         <f t="shared" si="2"/>
         <v>2.265625</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -935,8 +1244,14 @@
         <f t="shared" si="2"/>
         <v>2.265625</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -958,8 +1273,14 @@
         <f t="shared" si="2"/>
         <v>2.34765625</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -981,8 +1302,14 @@
         <f t="shared" si="2"/>
         <v>2.34765625</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1004,19 +1331,163 @@
         <f t="shared" si="2"/>
         <v>2.34765625</v>
       </c>
+      <c r="G13" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>1.55859375</v>
+      </c>
+      <c r="G17" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.78515625</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>2.35546875</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>1.55859375</v>
+      </c>
+      <c r="G18" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>1.55859375</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="top10" dxfId="7" priority="4" percent="1" rank="10"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="6" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="4" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Prepare for initial testing
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Test Name</t>
   </si>
@@ -316,6 +316,42 @@
   </si>
   <si>
     <t>10.03.txt</t>
+  </si>
+  <si>
+    <t>15.Start</t>
+  </si>
+  <si>
+    <t>15.Minute</t>
+  </si>
+  <si>
+    <t>15.Mix</t>
+  </si>
+  <si>
+    <t>15ST.1</t>
+  </si>
+  <si>
+    <t>15ST.2</t>
+  </si>
+  <si>
+    <t>15ST.3</t>
+  </si>
+  <si>
+    <t>15MT.1</t>
+  </si>
+  <si>
+    <t>15MT.2</t>
+  </si>
+  <si>
+    <t>15MT.3</t>
+  </si>
+  <si>
+    <t>15MX.1</t>
+  </si>
+  <si>
+    <t>15MX.2</t>
+  </si>
+  <si>
+    <t>15MX.3</t>
   </si>
 </sst>
 </file>
@@ -388,7 +424,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -708,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +811,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D19" si="0">1/3</f>
+        <f t="shared" ref="D2:D28" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -798,11 +844,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E19" si="1">C3/D3</f>
+        <f t="shared" ref="E3:E28" si="1">C3/D3</f>
         <v>2.30859375</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F19" si="2">AVERAGEIF(B:B,B3,E:E)</f>
+        <f t="shared" ref="F3:F28" si="2">AVERAGEIF(B:B,B3,E:E)</f>
         <v>2.296875</v>
       </c>
       <c r="G3" s="5">
@@ -1276,16 +1322,196 @@
         <v>47</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="2" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="2" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Snapshot - lost data
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -158,12 +158,101 @@
         </r>
       </text>
     </comment>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Start</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> meta-group.
+Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Minute</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Mix</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Test Name</t>
   </si>
@@ -352,6 +441,9 @@
   </si>
   <si>
     <t>15MX.3</t>
+  </si>
+  <si>
+    <t>11.07.txt</t>
   </si>
 </sst>
 </file>
@@ -757,7 +849,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1329,17 +1421,26 @@
       <c r="B20" t="s">
         <v>51</v>
       </c>
+      <c r="C20" s="1">
+        <v>0.8125</v>
+      </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8125</v>
+      </c>
+      <c r="G20" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1359,7 +1460,7 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1379,7 +1480,7 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Completed the 15.Start and 15.Minute series of tests, prepping for 15.Mix
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -252,10 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
-  <si>
-    <t>Test Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>Test Group</t>
   </si>
@@ -443,14 +440,32 @@
     <t>15MX.3</t>
   </si>
   <si>
-    <t>11.07.txt</t>
+    <t>11.23.txt</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>11.38.txt</t>
+  </si>
+  <si>
+    <t>11.53.txt</t>
+  </si>
+  <si>
+    <t>12.09.txt</t>
+  </si>
+  <si>
+    <t>12.25.txt</t>
+  </si>
+  <si>
+    <t>12.41.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -476,6 +491,29 @@
       <color indexed="81"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -500,19 +538,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -849,12 +892,12 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
@@ -865,39 +908,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>0.765625</v>
@@ -918,15 +961,15 @@
         <v>42537</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>0.76953125</v>
@@ -947,15 +990,15 @@
         <v>42537</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>0.76171875</v>
@@ -976,15 +1019,15 @@
         <v>42537</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>0.76171875</v>
@@ -1005,15 +1048,15 @@
         <v>42537</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>0.7421875</v>
@@ -1034,15 +1077,15 @@
         <v>42537</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>0.75390625</v>
@@ -1063,15 +1106,15 @@
         <v>42537</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>0.734375</v>
@@ -1092,15 +1135,15 @@
         <v>42537</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1">
         <v>0.7421875</v>
@@ -1121,15 +1164,15 @@
         <v>42537</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>0.7890625</v>
@@ -1150,15 +1193,15 @@
         <v>42537</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>0.77734375</v>
@@ -1179,15 +1222,15 @@
         <v>42537</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>0.796875</v>
@@ -1208,15 +1251,15 @@
         <v>42537</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="1">
         <v>0.7734375</v>
@@ -1237,15 +1280,15 @@
         <v>42537</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1">
         <v>0.77734375</v>
@@ -1266,15 +1309,15 @@
         <v>42538</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>0.76953125</v>
@@ -1295,15 +1338,15 @@
         <v>42538</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
       </c>
       <c r="C16" s="1">
         <v>0.75390625</v>
@@ -1324,15 +1367,15 @@
         <v>42538</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
         <v>0.7734375</v>
@@ -1353,15 +1396,15 @@
         <v>42537</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <v>0.78515625</v>
@@ -1382,15 +1425,15 @@
         <v>42537</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
         <v>0.76953125</v>
@@ -1411,18 +1454,18 @@
         <v>42538</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="1">
-        <v>0.8125</v>
+        <v>0.7265625</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
@@ -1430,25 +1473,28 @@
       </c>
       <c r="E20" s="3">
         <f t="shared" si="1"/>
-        <v>2.4375</v>
+        <v>2.1796875</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="2"/>
-        <v>0.8125</v>
+        <v>2.2421875</v>
       </c>
       <c r="G20" s="5">
         <v>42538</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.74609375</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
@@ -1456,19 +1502,28 @@
       </c>
       <c r="E21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.23828125</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="2"/>
-        <v>0.8125</v>
+        <v>2.2421875</v>
+      </c>
+      <c r="G21" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.76953125</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
@@ -1476,19 +1531,28 @@
       </c>
       <c r="E22" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.30859375</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="2"/>
-        <v>0.8125</v>
+        <v>2.2421875</v>
+      </c>
+      <c r="G22" s="6">
+        <v>42538</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.72265625</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
@@ -1496,19 +1560,28 @@
       </c>
       <c r="E23" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.16796875</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.234375</v>
+      </c>
+      <c r="G23" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.73828125</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
@@ -1516,19 +1589,28 @@
       </c>
       <c r="E24" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.21484375</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.234375</v>
+      </c>
+      <c r="G24" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.7734375</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
@@ -1536,19 +1618,25 @@
       </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.3203125</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.234375</v>
+      </c>
+      <c r="G25" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
@@ -1565,10 +1653,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
@@ -1585,10 +1673,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Finish the series of tests
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
+    <sheet name="15-Series" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -251,8 +252,107 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Grey</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Start</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> meta-group.
+Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Minute</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Mix</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Test Group</t>
   </si>
@@ -459,6 +559,18 @@
   </si>
   <si>
     <t>12.41.txt</t>
+  </si>
+  <si>
+    <t>12.57.txt</t>
+  </si>
+  <si>
+    <t>13.12.txt</t>
+  </si>
+  <si>
+    <t>14.20.txt</t>
+  </si>
+  <si>
+    <t>STDEV/Group</t>
   </si>
 </sst>
 </file>
@@ -559,7 +671,95 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -595,6 +795,62 @@
           <color rgb="FF00B050"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -891,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="G26:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,17 +1894,26 @@
       <c r="B26" t="s">
         <v>52</v>
       </c>
+      <c r="C26" s="1">
+        <v>0.8125</v>
+      </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.33203125</v>
+      </c>
+      <c r="G26" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1658,17 +1923,26 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
+      <c r="C27" s="1">
+        <v>0.70703125</v>
+      </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.12109375</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.33203125</v>
+      </c>
+      <c r="G27" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1678,29 +1952,386 @@
       <c r="B28" t="s">
         <v>52</v>
       </c>
+      <c r="C28" s="1">
+        <v>0.8125</v>
+      </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.33203125</v>
+      </c>
+      <c r="G28" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="4" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="2" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.7265625</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D10" si="0">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E10" si="1">C2/D2</f>
+        <v>2.1796875</v>
+      </c>
+      <c r="F2" s="3">
+        <f>AVERAGEIF(B:B,B2,E:E)</f>
+        <v>2.2421875</v>
+      </c>
+      <c r="G2" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="1"/>
+        <v>2.23828125</v>
+      </c>
+      <c r="F3" s="3">
+        <f>AVERAGEIF(B:B,B3,E:E)</f>
+        <v>2.2421875</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3">
+        <f>STDEV(C2:C4)</f>
+        <v>2.1513947450336336E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F4" s="3">
+        <f>AVERAGEIF(B:B,B4,E:E)</f>
+        <v>2.2421875</v>
+      </c>
+      <c r="G4" s="6">
+        <v>42538</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.72265625</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>2.16796875</v>
+      </c>
+      <c r="F5" s="3">
+        <f>AVERAGEIF(B:B,B5,E:E)</f>
+        <v>2.234375</v>
+      </c>
+      <c r="G5" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.73828125</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>2.21484375</v>
+      </c>
+      <c r="F6" s="3">
+        <f>AVERAGEIF(B:B,B6,E:E)</f>
+        <v>2.234375</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6">
+        <f>STDEV(C5:C7)</f>
+        <v>2.6009094212810127E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F7" s="3">
+        <f>AVERAGEIF(B:B,B7,E:E)</f>
+        <v>2.234375</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F8" s="3">
+        <f>AVERAGEIF(B:B,B8,E:E)</f>
+        <v>2.33203125</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.70703125</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>2.12109375</v>
+      </c>
+      <c r="F9" s="3">
+        <f>AVERAGEIF(B:B,B9,E:E)</f>
+        <v>2.33203125</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9">
+        <f>STDEV(C8:C10)</f>
+        <v>6.0892411203593344E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F10" s="3">
+        <f>AVERAGEIF(B:B,B10,E:E)</f>
+        <v>2.33203125</v>
+      </c>
+      <c r="G10" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C7 C10:C1048576">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:C9">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New test series: lessen_dropout
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>Test Group</t>
   </si>
@@ -571,6 +571,18 @@
   </si>
   <si>
     <t>STDEV/Group</t>
+  </si>
+  <si>
+    <t>Lessen_Dropout</t>
+  </si>
+  <si>
+    <t>LSDR.1</t>
+  </si>
+  <si>
+    <t>LSDR.2</t>
+  </si>
+  <si>
+    <t>LSDR.3</t>
   </si>
 </sst>
 </file>
@@ -671,7 +683,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -683,20 +695,14 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
-        </bottom>
-      </border>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -795,62 +801,6 @@
           <color rgb="FF00B050"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1145,16 +1095,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="G26:H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -1202,7 +1152,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D28" si="0">1/3</f>
+        <f t="shared" ref="D2:D31" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -1235,11 +1185,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E28" si="1">C3/D3</f>
+        <f t="shared" ref="E3:E31" si="1">C3/D3</f>
         <v>2.30859375</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F28" si="2">AVERAGEIF(B:B,B3,E:E)</f>
+        <f t="shared" ref="F3:F31" si="2">AVERAGEIF(B:B,B3,E:E)</f>
         <v>2.296875</v>
       </c>
       <c r="G3" s="5">
@@ -1972,6 +1922,75 @@
       </c>
       <c r="H28" s="5" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>42541</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>42541</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>42541</v>
       </c>
     </row>
   </sheetData>
@@ -1996,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2062,7 +2081,7 @@
         <v>2.1796875</v>
       </c>
       <c r="F2" s="3">
-        <f>AVERAGEIF(B:B,B2,E:E)</f>
+        <f t="shared" ref="F2:F10" si="2">AVERAGEIF(B:B,B2,E:E)</f>
         <v>2.2421875</v>
       </c>
       <c r="G2" s="5">
@@ -2091,7 +2110,7 @@
         <v>2.23828125</v>
       </c>
       <c r="F3" s="3">
-        <f>AVERAGEIF(B:B,B3,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.2421875</v>
       </c>
       <c r="G3" s="5">
@@ -2124,7 +2143,7 @@
         <v>2.30859375</v>
       </c>
       <c r="F4" s="3">
-        <f>AVERAGEIF(B:B,B4,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.2421875</v>
       </c>
       <c r="G4" s="6">
@@ -2153,7 +2172,7 @@
         <v>2.16796875</v>
       </c>
       <c r="F5" s="3">
-        <f>AVERAGEIF(B:B,B5,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.234375</v>
       </c>
       <c r="G5" s="5">
@@ -2182,7 +2201,7 @@
         <v>2.21484375</v>
       </c>
       <c r="F6" s="3">
-        <f>AVERAGEIF(B:B,B6,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.234375</v>
       </c>
       <c r="G6" s="5">
@@ -2215,7 +2234,7 @@
         <v>2.3203125</v>
       </c>
       <c r="F7" s="3">
-        <f>AVERAGEIF(B:B,B7,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.234375</v>
       </c>
       <c r="G7" s="5">
@@ -2244,7 +2263,7 @@
         <v>2.4375</v>
       </c>
       <c r="F8" s="3">
-        <f>AVERAGEIF(B:B,B8,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.33203125</v>
       </c>
       <c r="G8" s="5">
@@ -2273,7 +2292,7 @@
         <v>2.12109375</v>
       </c>
       <c r="F9" s="3">
-        <f>AVERAGEIF(B:B,B9,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.33203125</v>
       </c>
       <c r="G9" s="5">
@@ -2306,7 +2325,7 @@
         <v>2.4375</v>
       </c>
       <c r="F10" s="3">
-        <f>AVERAGEIF(B:B,B10,E:E)</f>
+        <f t="shared" si="2"/>
         <v>2.33203125</v>
       </c>
       <c r="G10" s="5">

</xml_diff>

<commit_message>
Snapshot - data loss because I'm an IDIOT
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>Test Group</t>
   </si>
@@ -1235,7 +1235,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2155,20 +2155,29 @@
       <c r="B32" t="s">
         <v>79</v>
       </c>
+      <c r="C32" s="1">
+        <v>0.8046875</v>
+      </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E32" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4140625</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.48281249999999998</v>
+      </c>
+      <c r="G32" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -2185,10 +2194,13 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.48281249999999998</v>
+      </c>
+      <c r="G33" s="5">
+        <v>42541</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2205,10 +2217,10 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.48281249999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>83</v>
       </c>
@@ -2225,10 +2237,10 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ref="F35:F36" si="4">AVERAGEIF(B:B,B35,E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.48281249999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -2245,7 +2257,7 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.48281249999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run a couple tests and tweak some comments for clarity
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F32" s="3">
         <f>AVERAGEIF(B:B,B33,E:E)</f>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
       <c r="G32" s="5">
         <v>42541</v>
@@ -2245,17 +2245,20 @@
       <c r="B33" t="s">
         <v>79</v>
       </c>
+      <c r="C33" s="1">
+        <v>0.71875</v>
+      </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.15625</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" ref="F33:F34" si="3">AVERAGEIF(B:B,B34,E:E)</f>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
       <c r="G33" s="5">
         <v>42541</v>
@@ -2278,7 +2281,7 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -2298,7 +2301,7 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ref="F35:F36" si="5">AVERAGEIF(B:B,B35,E:E)</f>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2318,7 +2321,7 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2338,7 +2341,7 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ref="F37" si="7">AVERAGEIF(B:B,B37,E:E)</f>
-        <v>0</v>
+        <v>0.43125000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete first run through of experiments
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2341,17 +2341,23 @@
       <c r="B38" t="s">
         <v>90</v>
       </c>
+      <c r="C38" s="1">
+        <v>0.75390625</v>
+      </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" ref="E38" si="8">C38/D38</f>
-        <v>0</v>
+        <v>2.26171875</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" ref="F38:F40" si="9">AVERAGEIF(B:B,B38,E:E)</f>
-        <v>0</v>
+        <v>2.19921875</v>
+      </c>
+      <c r="G38" s="5">
+        <v>42542</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -2361,17 +2367,23 @@
       <c r="B39" t="s">
         <v>90</v>
       </c>
+      <c r="C39" s="1">
+        <v>0.69921875</v>
+      </c>
       <c r="D39" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E39" s="3">
         <f t="shared" ref="E39:E40" si="10">C39/D39</f>
-        <v>0</v>
+        <v>2.09765625</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.19921875</v>
+      </c>
+      <c r="G39" s="5">
+        <v>42542</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -2381,17 +2393,23 @@
       <c r="B40" t="s">
         <v>90</v>
       </c>
+      <c r="C40" s="1">
+        <v>0.74609375</v>
+      </c>
       <c r="D40" s="1">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.23828125</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.19921875</v>
+      </c>
+      <c r="G40" s="5">
+        <v>42542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes in loading weights code
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
   <si>
     <t>Test Group</t>
   </si>
@@ -712,9 +712,6 @@
     <t>17.49.txt</t>
   </si>
   <si>
-    <t>MTRN1</t>
-  </si>
-  <si>
     <t>MTRN1.1</t>
   </si>
   <si>
@@ -722,6 +719,18 @@
   </si>
   <si>
     <t>MTRN1.3</t>
+  </si>
+  <si>
+    <t>09.35.txt</t>
+  </si>
+  <si>
+    <t>MTRN1.2.1</t>
+  </si>
+  <si>
+    <t>MTRN1.2.2</t>
+  </si>
+  <si>
+    <t>MTRN1.2.3</t>
   </si>
 </sst>
 </file>
@@ -822,7 +831,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1244,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1330,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D40" si="0">1/3</f>
+        <f t="shared" ref="D2:D43" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -2336,7 +2365,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
         <v>90</v>
@@ -2353,16 +2382,19 @@
         <v>2.26171875</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" ref="F38:F40" si="9">AVERAGEIF(B:B,B38,E:E)</f>
+        <f t="shared" ref="F38:F43" si="9">AVERAGEIF(B:B,B38,E:E)</f>
         <v>2.19921875</v>
       </c>
       <c r="G38" s="5">
         <v>42542</v>
       </c>
+      <c r="H38" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" t="s">
         <v>90</v>
@@ -2385,10 +2417,13 @@
       <c r="G39" s="5">
         <v>42542</v>
       </c>
+      <c r="H39" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
         <v>90</v>
@@ -2411,17 +2446,89 @@
       <c r="G40" s="5">
         <v>42542</v>
       </c>
+      <c r="H40" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" ref="E41:E43" si="11">C41/D41</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>42542</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>42542</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>42542</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="12" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="11" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="10" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="12" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2756,20 +2863,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="8" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="7" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="6" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="4" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="6" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Prep log for building defaults
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -336,6 +336,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">default:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Create a default set of weights and a model for testing to see which songs are mis-identified every time.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -440,7 +462,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
   <si>
     <t>Test Group</t>
   </si>
@@ -734,6 +756,18 @@
   </si>
   <si>
     <t>13.14.txt</t>
+  </si>
+  <si>
+    <t>default.1</t>
+  </si>
+  <si>
+    <t>default.2</t>
+  </si>
+  <si>
+    <t>default.3</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -834,37 +868,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1276,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42:H43"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1337,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D43" si="0">1/3</f>
+        <f t="shared" ref="D2:D46" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -2385,7 +2389,7 @@
         <v>2.26171875</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" ref="F38:F43" si="9">AVERAGEIF(B:B,B38,E:E)</f>
+        <f t="shared" ref="F38:F46" si="9">AVERAGEIF(B:B,B38,E:E)</f>
         <v>2.19921875</v>
       </c>
       <c r="G38" s="5">
@@ -2540,16 +2544,76 @@
         <v>97</v>
       </c>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" ref="E44:E46" si="12">C44/D44</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="14" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="12" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2884,20 +2948,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="10" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="9" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="6" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Prep for new training
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
   <si>
     <t>Test Group</t>
   </si>
@@ -931,6 +931,18 @@
   </si>
   <si>
     <t>20.19.txt</t>
+  </si>
+  <si>
+    <t>20Sec1Minute</t>
+  </si>
+  <si>
+    <t>2S1M.0.0</t>
+  </si>
+  <si>
+    <t>2S1M.0.1</t>
+  </si>
+  <si>
+    <t>2S1M.0.2</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1048,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1428,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,7 +1517,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D55" si="0">1/3</f>
+        <f t="shared" ref="D2:D58" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -2885,7 +2917,7 @@
         <v>2.5078125</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" ref="F50:F55" si="14">AVERAGEIF(B:B,B50,E:E)</f>
+        <f t="shared" ref="F50:F56" si="14">AVERAGEIF(B:B,B50,E:E)</f>
         <v>2.370159313959233</v>
       </c>
       <c r="G50" s="5">
@@ -3041,16 +3073,76 @@
         <v>116</v>
       </c>
     </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" ref="E56:E58" si="15">C56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" ref="F56:F58" si="16">AVERAGEIF(B:B,B56,E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3386,20 +3478,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix crash when a badly-timed song is the wrong length
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="123">
   <si>
     <t>Test Group</t>
   </si>
@@ -965,6 +965,12 @@
   </si>
   <si>
     <t>2S1M.0.2</t>
+  </si>
+  <si>
+    <t>12.10.txt</t>
+  </si>
+  <si>
+    <t>2S1Mo.0.0</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1076,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1482,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,7 +1565,7 @@
         <v>0.765625</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D58" si="0">1/3</f>
+        <f t="shared" ref="D2:D59" si="0">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E2" s="3">
@@ -3097,7 +3123,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
         <v>117</v>
@@ -3115,12 +3141,18 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" ref="F56:F58" si="16">AVERAGEIF(B:B,B56,E:E)</f>
-        <v>0.82071713123663415</v>
+        <v>0.61553784842747561</v>
+      </c>
+      <c r="G56" s="5">
+        <v>42549</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" t="s">
         <v>117</v>
@@ -3135,12 +3167,12 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" si="16"/>
-        <v>0.82071713123663415</v>
+        <v>0.61553784842747561</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
         <v>117</v>
@@ -3155,19 +3187,39 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" si="16"/>
-        <v>0.82071713123663415</v>
+        <v>0.61553784842747561</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" ref="E59" si="17">C59/D59</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" ref="F59" si="18">AVERAGEIF(B:B,B59,E:E)</f>
+        <v>0.61553784842747561</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3503,20 +3555,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="5" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finish experiments for the day
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -783,7 +783,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="156">
   <si>
     <t>Test Group</t>
   </si>
@@ -1248,6 +1248,9 @@
   </si>
   <si>
     <t>INS5.0.2</t>
+  </si>
+  <si>
+    <t>16.29.txt</t>
   </si>
 </sst>
 </file>
@@ -1804,7 +1807,7 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4013,7 +4016,13 @@
       </c>
       <c r="F76" s="3">
         <f t="shared" si="27"/>
-        <v>0.38200000000000006</v>
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="G76" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -4023,17 +4032,26 @@
       <c r="B77" t="s">
         <v>151</v>
       </c>
+      <c r="C77" s="1">
+        <v>0.34399999999999997</v>
+      </c>
       <c r="D77" s="1">
         <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1.032</v>
       </c>
       <c r="F77" s="3">
         <f t="shared" si="27"/>
-        <v>0.38200000000000006</v>
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="G77" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -4043,17 +4061,26 @@
       <c r="B78" t="s">
         <v>151</v>
       </c>
+      <c r="C78" s="1">
+        <v>0.36799999999999999</v>
+      </c>
       <c r="D78" s="1">
         <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="F78" s="3">
         <f t="shared" si="27"/>
-        <v>0.38200000000000006</v>
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="G78" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished up the poster stuff, and did some stuff in the experiment log to have nice charts
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
-    <sheet name="15-Series" sheetId="2" r:id="rId2"/>
+    <sheet name="GenreID" sheetId="3" r:id="rId2"/>
+    <sheet name="15-Series" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -723,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -732,7 +733,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Instrument7:
+          <t xml:space="preserve">Instrument8:
 </t>
         </r>
         <r>
@@ -741,12 +742,8 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>More tweaks of neural network shape. This one is a series of layers of decreasing powers of two neurons.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B84" authorId="0">
-      <text>
+          <t xml:space="preserve">Testing the Instrument series using the same network shape as </t>
+        </r>
         <r>
           <rPr>
             <b/>
@@ -754,16 +751,16 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Instrument7:
+          <t>Instrument7</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">, but with an input window of twice the size.
 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>More tweaks of neural network shape. This one is a series of layers of decreasing powers of two neurons.</t>
         </r>
       </text>
     </comment>
@@ -786,6 +783,594 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t>Midpoint 3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Feeds raw samples from :30-:40 into NN, attempting to map the song into one of three genres: art, pop, or traditional.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Midpoint 3
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Feeds raw samples from :00-:10 into NN, attempting to map the song into one of three genres: art, pop, or traditional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>StartDouble3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Reads from :00 to :20, feeds raw samples into the neural network, and then attempts to categorize them into three genres: art, pop, or traditional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">NewShape3
+Testing the same thing as StartDouble3, but with the initial layer of the NN widened out to 2* size.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">DeeperNN
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Testing the same thing as NewShape3, but with an additional 64-neuron, tanh layer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">MidpointWide
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Testing the same thing as NewShape3, but using the :10-:30 chunk instead of :00-:20
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Start</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> meta-group.
+Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Minute</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Mix</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Lessen_Dropout
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Testing the normal neural network layout with the 'dropout' setting dropped from 0.5 to 0.25</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">15.Mix.exNULL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Data loss problem with this one - I'm leaving the record in here, but culling it from the rest of the 15.Mix.extended series.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">15.Mix.extended
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>A trial of the 15.Mix using a batch size larger than the dataset - rolling over the end of the dataset will force rebuilding of some songs, which will allow us to artificially incrase the size of the dataset by a large amount.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">MTRN1:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Multiple trainings on the same neural network.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">default:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Create a default set of weights and a model for testing to see which songs are mis-identified every time.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newCategories:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Using the data from the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>default</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> test, I shuffled around some of the ways that genres were mapped to meta-genres. Testing the results here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">newDataSet:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Testing the same thing as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newCategories</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>, utilizing an updated data set that includes more music in the 'art' meta-genre.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newDataSet.1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Secondary training on the networks produced by </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newDataSet</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Unhandled exception in the </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>next_batch</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> code crashed the run after the first one - spent a while fixing it.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">20Sec1Minute:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Feeds in samples 20 seconds long, non-randomized, starting 1 minute into the song.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">BiggerNN:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Using a significantly-larger neural network with the 20-seconds-at-1-minute input - added another layer, and gave it a pyramid shape, so 256-128-64-end.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">The120:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Limiting the amount of songs being fed in in an effort to reduce the amount of overfitting.
+Which, with only 120 samples, probably won't work. Dang.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">The120Repeat:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Use the samples from </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>The120</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>, but set to randomize and run through them all multiple times.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Grey</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t>15.Start</t>
         </r>
         <r>
@@ -871,7 +1456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="170">
   <si>
     <t>Test Group</t>
   </si>
@@ -1369,6 +1954,18 @@
   </si>
   <si>
     <t>14.28.txt</t>
+  </si>
+  <si>
+    <t>INS8.0.0</t>
+  </si>
+  <si>
+    <t>Instrument8</t>
+  </si>
+  <si>
+    <t>INS8.0.1</t>
+  </si>
+  <si>
+    <t>INS8.0.2</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +2077,119 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1607,6 +2316,1263 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GenreID!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>GenreID!$B$2:$B$71</c:f>
+              <c:strCache>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>Midpoint 3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Midpoint 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Midpoint 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Start 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Start 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Start 3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>StartDouble3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>StartDouble3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>StartDouble3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NewShape3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NewShape3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NewShape3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>DeeperNN</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>DeeperNN</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>DeeperNN</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>MidpointWide</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>MidpointWide</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>MidpointWide</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.Start</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.Start</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15.Start</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.Minute</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.Minute</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15.Minute</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15.Mix</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15.Mix</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15.Mix</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Lessen_Dropout</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Lessen_Dropout</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Lessen_Dropout</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.Mix.exNULL</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.Mix.extended</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15.Mix.extended</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15.Mix.extended</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15.Mix.extended</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.Mix.extended</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>MTRN1.1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>MTRN1.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>MTRN1.1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>MTRN1.2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>MTRN1.2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>MTRN1.2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>default</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>default</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>default</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>newCategories</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>newCategories</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>newCategories</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>newDataSet</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>newDataSet</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>newDataSet</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>newDataSet.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>newDataSet.1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>newDataSet.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>20Sec1Minute</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>20Sec1Minute</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>20Sec1Minute</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>20Sec1Minute</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>BiggerNN</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>BiggerNN</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>BiggerNN</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>The120</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>The120</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>The120</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>The120Repeat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>GenreID!$C$2:$C$71</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="70"/>
+                <c:pt idx="0">
+                  <c:v>0.765625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76171875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76171875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7421875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75390625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.734375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7421875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7890625</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77734375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.796875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7734375</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.77734375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.75390625</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7734375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.78515625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.7265625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.74609375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.72265625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.73828125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.7734375</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.70703125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.703125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.77734375</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.75390625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.73828125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.71875</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.79296875</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.71484375</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.73046875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.74609375</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.75390625</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69921875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.74609375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.80078125</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.734375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.7265625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.76171875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.94921875</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.91796875</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.8359375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.7734375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.760784313959233</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.828125</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.828125</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.850980392858093</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.820717131236634</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.835294117880802</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.837301586355481</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.818897638264603</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.861111112057216</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.873015873961978</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.858299595383014</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.300000003973642</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.333333339293797</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.200000002980232</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.40000000099341</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.233333339293797</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.200000002980232</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.466666666666666</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.266666670640309</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.400000001986821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2019016320"/>
+        <c:axId val="-2019034608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2019016320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2019034608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2019034608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2019016320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>395817</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>332317</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1872,10 +3838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3815,7 +5781,7 @@
         <v>0.23333333929379699</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:D84" si="25">1/3</f>
+        <f t="shared" ref="D67:D87" si="25">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="E67" s="3">
@@ -3881,7 +5847,7 @@
         <v>1.3999999999999981</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" ref="F69:F79" si="27">AVERAGEIF(B:B,B69,E:E)</f>
+        <f t="shared" ref="F69:F78" si="27">AVERAGEIF(B:B,B69,E:E)</f>
         <v>0.98333334128061756</v>
       </c>
       <c r="G69" s="5">
@@ -4170,7 +6136,7 @@
         <v>0.90600000000000003</v>
       </c>
       <c r="F79" s="3">
-        <f t="shared" ref="F79:F82" si="31">AVERAGEIF(B:B,B79,E:E)</f>
+        <f t="shared" ref="F79:F81" si="31">AVERAGEIF(B:B,B79,E:E)</f>
         <v>0.96200000000000008</v>
       </c>
       <c r="G79" s="5">
@@ -4257,7 +6223,7 @@
         <v>1.1280000000000001</v>
       </c>
       <c r="F82" s="3">
-        <f t="shared" ref="F82:F84" si="33">AVERAGEIF(B:B,B82,E:E)</f>
+        <f t="shared" ref="F82:F85" si="33">AVERAGEIF(B:B,B82,E:E)</f>
         <v>1.0640000000000001</v>
       </c>
       <c r="G82" s="5">
@@ -4325,16 +6291,79 @@
         <v>165</v>
       </c>
     </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85" t="s">
+        <v>167</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="25"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E85" s="3">
+        <f t="shared" ref="E85:E87" si="34">C85/D85</f>
+        <v>1.0200000000000002</v>
+      </c>
+      <c r="F85" s="3">
+        <f t="shared" ref="F85:F87" si="35">AVERAGEIF(B:B,B85,E:E)</f>
+        <v>0.34000000000000008</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" t="s">
+        <v>167</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="25"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E86" s="3">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="F86" s="3">
+        <f t="shared" si="35"/>
+        <v>0.34000000000000008</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>169</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="25"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E87" s="3">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="3">
+        <f t="shared" si="35"/>
+        <v>0.34000000000000008</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="19" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="18" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="17" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4345,6 +6374,2091 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.765625</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D66" si="0">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2/D2</f>
+        <v>2.296875</v>
+      </c>
+      <c r="F2" s="3">
+        <f>AVERAGEIF(B:B,B2,E:E)</f>
+        <v>2.296875</v>
+      </c>
+      <c r="G2" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E66" si="1">C3/D3</f>
+        <v>2.30859375</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F31" si="2">AVERAGEIF(B:B,B3,E:E)</f>
+        <v>2.296875</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.76171875</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.28515625</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>2.296875</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.76171875</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>2.28515625</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G5" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.7421875</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2265625</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.75390625</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>2.26171875</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.734375</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>2.203125</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>2.265625</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.7421875</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2265625</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.265625</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.7890625</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3671875</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>2.265625</v>
+      </c>
+      <c r="G10" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.77734375</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>2.34765625</v>
+      </c>
+      <c r="G11" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.796875</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>2.390625</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>2.34765625</v>
+      </c>
+      <c r="G12" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>2.34765625</v>
+      </c>
+      <c r="G13" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.77734375</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>2.30078125</v>
+      </c>
+      <c r="G14" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>2.30078125</v>
+      </c>
+      <c r="G15" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.75390625</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>2.26171875</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>2.30078125</v>
+      </c>
+      <c r="G16" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>2.328125</v>
+      </c>
+      <c r="G17" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.78515625</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>2.35546875</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>2.328125</v>
+      </c>
+      <c r="G18" s="5">
+        <v>42537</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>2.328125</v>
+      </c>
+      <c r="G19" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.7265625</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1796875</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2421875</v>
+      </c>
+      <c r="G20" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>2.23828125</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2421875</v>
+      </c>
+      <c r="G21" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2421875</v>
+      </c>
+      <c r="G22" s="6">
+        <v>42538</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.72265625</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>2.16796875</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G23" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.73828125</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>2.21484375</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G24" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G25" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G26" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.70703125</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="1"/>
+        <v>2.12109375</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G27" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G28" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.703125</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="1"/>
+        <v>2.109375</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G29" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.77734375</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="1"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G30" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.75390625</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="1"/>
+        <v>2.26171875</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G31" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.73828125</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>2.21484375</v>
+      </c>
+      <c r="F32" s="3">
+        <f>AVERAGEIF(B:B,B33,E:E)</f>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G32" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>2.15625</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" ref="F33:F34" si="3">AVERAGEIF(B:B,B34,E:E)</f>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G33" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.79296875</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>2.37890625</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="3"/>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G34" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.71484375</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="1"/>
+        <v>2.14453125</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" ref="F35:F71" si="4">AVERAGEIF(B:B,B35,E:E)</f>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G35" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.73046875</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="1"/>
+        <v>2.19140625</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G36" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="1"/>
+        <v>2.23828125</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2218749999999998</v>
+      </c>
+      <c r="G37" s="5">
+        <v>42541</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.75390625</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="1"/>
+        <v>2.26171875</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="4"/>
+        <v>2.19921875</v>
+      </c>
+      <c r="G38" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.69921875</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="1"/>
+        <v>2.09765625</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="4"/>
+        <v>2.19921875</v>
+      </c>
+      <c r="G39" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="1"/>
+        <v>2.23828125</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="4"/>
+        <v>2.19921875</v>
+      </c>
+      <c r="G40" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.80078125</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="1"/>
+        <v>2.40234375</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="4"/>
+        <v>2.3046875</v>
+      </c>
+      <c r="G41" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="4"/>
+        <v>2.3046875</v>
+      </c>
+      <c r="G42" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.734375</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="1"/>
+        <v>2.203125</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="4"/>
+        <v>2.3046875</v>
+      </c>
+      <c r="G43" s="5">
+        <v>42542</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.7265625</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1796875</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G44" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G45" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.76171875</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="1"/>
+        <v>2.28515625</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2578125</v>
+      </c>
+      <c r="G46" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="1"/>
+        <v>2.8125</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8046875</v>
+      </c>
+      <c r="G47" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.94921875</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="1"/>
+        <v>2.84765625</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8046875</v>
+      </c>
+      <c r="G48" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.91796875</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E49" s="3">
+        <f t="shared" si="1"/>
+        <v>2.75390625</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8046875</v>
+      </c>
+      <c r="G49" s="5">
+        <v>42543</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.8359375</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5078125</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="4"/>
+        <v>2.370159313959233</v>
+      </c>
+      <c r="G50" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E51" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="4"/>
+        <v>2.370159313959233</v>
+      </c>
+      <c r="G51" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.76078431395923296</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E52" s="3">
+        <f t="shared" si="1"/>
+        <v>2.2823529418776989</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="4"/>
+        <v>2.370159313959233</v>
+      </c>
+      <c r="G52" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.828125</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E53" s="3">
+        <f t="shared" si="1"/>
+        <v>2.484375</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="4"/>
+        <v>2.507230392858093</v>
+      </c>
+      <c r="G53" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.828125</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E54" s="3">
+        <f t="shared" si="1"/>
+        <v>2.484375</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="4"/>
+        <v>2.507230392858093</v>
+      </c>
+      <c r="G54" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0.85098039285809302</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="1"/>
+        <v>2.552941178574279</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="4"/>
+        <v>2.507230392858093</v>
+      </c>
+      <c r="G55" s="5">
+        <v>42548</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.82071713123663403</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E56" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4621513937099024</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="4"/>
+        <v>2.48415785530314</v>
+      </c>
+      <c r="G56" s="5">
+        <v>42549</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.83529411788080199</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5058823536424062</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="4"/>
+        <v>2.48415785530314</v>
+      </c>
+      <c r="G57" s="5">
+        <v>42549</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0.83730158635548102</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E58" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5119047590664434</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" si="4"/>
+        <v>2.48415785530314</v>
+      </c>
+      <c r="G58" s="5">
+        <v>42549</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0.81889763826460304</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E59" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4566929147938095</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="4"/>
+        <v>2.48415785530314</v>
+      </c>
+      <c r="G59" s="5">
+        <v>42549</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.86111111205721602</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E60" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5833333361716484</v>
+      </c>
+      <c r="F60" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5924265814022083</v>
+      </c>
+      <c r="G60" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0.873015873961978</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E61" s="3">
+        <f t="shared" si="1"/>
+        <v>2.619047621885934</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5924265814022083</v>
+      </c>
+      <c r="G61" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0.85829959538301404</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" si="1"/>
+        <v>2.5748987861490424</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="4"/>
+        <v>2.5924265814022083</v>
+      </c>
+      <c r="G62" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0.30000000397364202</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E63" s="3">
+        <f t="shared" si="1"/>
+        <v>0.90000001192092605</v>
+      </c>
+      <c r="F63" s="3">
+        <f t="shared" si="4"/>
+        <v>0.83333334624767108</v>
+      </c>
+      <c r="G63" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0.33333333929379699</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E64" s="3">
+        <f t="shared" si="1"/>
+        <v>1.000000017881391</v>
+      </c>
+      <c r="F64" s="3">
+        <f t="shared" si="4"/>
+        <v>0.83333334624767108</v>
+      </c>
+      <c r="G64" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0.20000000298023199</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E65" s="3">
+        <f t="shared" si="1"/>
+        <v>0.60000000894069605</v>
+      </c>
+      <c r="F65" s="3">
+        <f t="shared" si="4"/>
+        <v>0.83333334624767108</v>
+      </c>
+      <c r="G65" s="5">
+        <v>42550</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0.40000000099340999</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E66" s="3">
+        <f t="shared" si="1"/>
+        <v>1.20000000298023</v>
+      </c>
+      <c r="F66" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G66" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0.23333333929379699</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D71" si="5">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E67" s="3">
+        <f t="shared" ref="E67:E71" si="6">C67/D67</f>
+        <v>0.70000001788139099</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G67" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>133</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0.20000000298023199</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E68" s="3">
+        <f t="shared" si="6"/>
+        <v>0.60000000894069605</v>
+      </c>
+      <c r="F68" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G68" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E69" s="3">
+        <f t="shared" si="6"/>
+        <v>1.3999999999999981</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G69" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" t="s">
+        <v>133</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0.26666667064030902</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E70" s="3">
+        <f t="shared" si="6"/>
+        <v>0.80000001192092707</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G70" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0.40000000198682101</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E71" s="3">
+        <f t="shared" si="6"/>
+        <v>1.2000000059604632</v>
+      </c>
+      <c r="F71" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98333334128061756</v>
+      </c>
+      <c r="G71" s="5">
+        <v>42551</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E71">
+    <cfRule type="top10" dxfId="7" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F71">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C71">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -4670,20 +8784,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="14" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Getting graphs, thanks Excel
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -3840,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6311,7 +6311,10 @@
       </c>
       <c r="F85" s="3">
         <f t="shared" ref="F85:F87" si="35">AVERAGEIF(B:B,B85,E:E)</f>
-        <v>0.34000000000000008</v>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="G85" s="5">
+        <v>42559</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -6321,17 +6324,23 @@
       <c r="B86" t="s">
         <v>167</v>
       </c>
+      <c r="C86" s="1">
+        <v>0.35</v>
+      </c>
       <c r="D86" s="1">
         <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E86" s="3">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="F86" s="3">
         <f t="shared" si="35"/>
-        <v>0.34000000000000008</v>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="G86" s="5">
+        <v>42559</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -6351,7 +6360,10 @@
       </c>
       <c r="F87" s="3">
         <f t="shared" si="35"/>
-        <v>0.34000000000000008</v>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="G87" s="5">
+        <v>42559</v>
       </c>
     </row>
   </sheetData>
@@ -6377,8 +6389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Log experiment over here bc why would git ever cooperate
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -1456,7 +1456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="171">
   <si>
     <t>Test Group</t>
   </si>
@@ -1966,6 +1966,9 @@
   </si>
   <si>
     <t>INS8.0.2</t>
+  </si>
+  <si>
+    <t>12.21.txt</t>
   </si>
 </sst>
 </file>
@@ -2077,119 +2080,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2308,6 +2199,52 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -2333,7 +2270,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2842,11 +2778,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2019016320"/>
-        <c:axId val="-2019034608"/>
+        <c:axId val="2097008432"/>
+        <c:axId val="2097012032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019016320"/>
+        <c:axId val="2097008432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2889,7 +2825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019034608"/>
+        <c:crossAx val="2097012032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2897,7 +2833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019034608"/>
+        <c:axId val="2097012032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2948,7 +2884,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019016320"/>
+        <c:crossAx val="2097008432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3841,7 +3777,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6223,7 +6159,7 @@
         <v>1.1280000000000001</v>
       </c>
       <c r="F82" s="3">
-        <f t="shared" ref="F82:F85" si="33">AVERAGEIF(B:B,B82,E:E)</f>
+        <f t="shared" ref="F82:F84" si="33">AVERAGEIF(B:B,B82,E:E)</f>
         <v>1.0640000000000001</v>
       </c>
       <c r="G82" s="5">
@@ -6311,10 +6247,13 @@
       </c>
       <c r="F85" s="3">
         <f t="shared" ref="F85:F87" si="35">AVERAGEIF(B:B,B85,E:E)</f>
-        <v>0.69000000000000006</v>
+        <v>1.0440000000000003</v>
       </c>
       <c r="G85" s="5">
         <v>42559</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -6337,10 +6276,13 @@
       </c>
       <c r="F86" s="3">
         <f t="shared" si="35"/>
-        <v>0.69000000000000006</v>
+        <v>1.0440000000000003</v>
       </c>
       <c r="G86" s="5">
         <v>42559</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -6350,32 +6292,38 @@
       <c r="B87" t="s">
         <v>167</v>
       </c>
+      <c r="C87" s="1">
+        <v>0.35399999999999998</v>
+      </c>
       <c r="D87" s="1">
         <f t="shared" si="25"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E87" s="3">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="F87" s="3">
         <f t="shared" si="35"/>
-        <v>0.69000000000000006</v>
+        <v>1.0440000000000003</v>
       </c>
       <c r="G87" s="5">
         <v>42559</v>
       </c>
+      <c r="H87" s="5" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="19" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="18" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="17" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8453,14 +8401,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="7" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8796,20 +8744,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="15" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="14" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix glitch in log
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -3811,7 +3811,7 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6011,16 +6011,15 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" ref="E76:E78" si="29">C76/D76</f>
-        <v>1.1460000000000001</v>
+        <v>1.528</v>
       </c>
       <c r="F76" s="3">
         <f t="shared" si="27"/>
-        <v>1.0940000000000001</v>
+        <v>1.4586666666666666</v>
       </c>
       <c r="G76" s="5">
         <v>42557</v>
@@ -6040,16 +6039,15 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="29"/>
-        <v>1.032</v>
+        <v>1.3759999999999999</v>
       </c>
       <c r="F77" s="3">
         <f t="shared" si="27"/>
-        <v>1.0940000000000001</v>
+        <v>1.4586666666666666</v>
       </c>
       <c r="G77" s="5">
         <v>42557</v>
@@ -6069,16 +6067,15 @@
         <v>0.36799999999999999</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="29"/>
-        <v>1.1040000000000001</v>
+        <v>1.472</v>
       </c>
       <c r="F78" s="3">
         <f t="shared" si="27"/>
-        <v>1.0940000000000001</v>
+        <v>1.4586666666666666</v>
       </c>
       <c r="G78" s="5">
         <v>42557</v>
@@ -6098,16 +6095,15 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E79" s="3">
         <f t="shared" ref="E79:E81" si="30">C79/D79</f>
-        <v>0.90600000000000003</v>
+        <v>1.208</v>
       </c>
       <c r="F79" s="3">
         <f t="shared" ref="F79:F81" si="31">AVERAGEIF(B:B,B79,E:E)</f>
-        <v>0.96200000000000008</v>
+        <v>1.2826666666666666</v>
       </c>
       <c r="G79" s="5">
         <v>42558</v>
@@ -6127,16 +6123,15 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E80" s="3">
         <f t="shared" si="30"/>
-        <v>1.032</v>
+        <v>1.3759999999999999</v>
       </c>
       <c r="F80" s="3">
         <f t="shared" si="31"/>
-        <v>0.96200000000000008</v>
+        <v>1.2826666666666666</v>
       </c>
       <c r="G80" s="5">
         <v>42558</v>
@@ -6156,16 +6151,15 @@
         <v>0.316</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E81" s="3">
         <f t="shared" si="30"/>
-        <v>0.94800000000000006</v>
+        <v>1.264</v>
       </c>
       <c r="F81" s="3">
         <f t="shared" si="31"/>
-        <v>0.96200000000000008</v>
+        <v>1.2826666666666666</v>
       </c>
       <c r="G81" s="5">
         <v>42558</v>
@@ -6185,16 +6179,15 @@
         <v>0.376</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E82" s="3">
         <f t="shared" ref="E82:E84" si="32">C82/D82</f>
-        <v>1.1280000000000001</v>
+        <v>1.504</v>
       </c>
       <c r="F82" s="3">
         <f t="shared" ref="F82:F84" si="33">AVERAGEIF(B:B,B82,E:E)</f>
-        <v>1.0640000000000001</v>
+        <v>1.4186666666666667</v>
       </c>
       <c r="G82" s="5">
         <v>42558</v>
@@ -6214,16 +6207,15 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E83" s="3">
         <f t="shared" si="32"/>
-        <v>1.0140000000000002</v>
+        <v>1.3520000000000001</v>
       </c>
       <c r="F83" s="3">
         <f t="shared" si="33"/>
-        <v>1.0640000000000001</v>
+        <v>1.4186666666666667</v>
       </c>
       <c r="G83" s="5">
         <v>42558</v>
@@ -6243,16 +6235,15 @@
         <v>0.35</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E84" s="3">
         <f t="shared" si="32"/>
-        <v>1.05</v>
+        <v>1.4</v>
       </c>
       <c r="F84" s="3">
         <f t="shared" si="33"/>
-        <v>1.0640000000000001</v>
+        <v>1.4186666666666667</v>
       </c>
       <c r="G84" s="5">
         <v>42558</v>
@@ -6272,16 +6263,15 @@
         <v>0.34</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E85" s="3">
         <f t="shared" ref="E85:E87" si="34">C85/D85</f>
-        <v>1.0200000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="F85" s="3">
         <f t="shared" ref="F85:F90" si="35">AVERAGEIF(B:B,B85,E:E)</f>
-        <v>1.0440000000000003</v>
+        <v>1.3920000000000001</v>
       </c>
       <c r="G85" s="5">
         <v>42559</v>
@@ -6301,16 +6291,15 @@
         <v>0.35</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E86" s="3">
         <f t="shared" si="34"/>
-        <v>1.05</v>
+        <v>1.4</v>
       </c>
       <c r="F86" s="3">
         <f t="shared" si="35"/>
-        <v>1.0440000000000003</v>
+        <v>1.3920000000000001</v>
       </c>
       <c r="G86" s="5">
         <v>42559</v>
@@ -6330,16 +6319,15 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E87" s="3">
         <f t="shared" si="34"/>
-        <v>1.0620000000000001</v>
+        <v>1.4159999999999999</v>
       </c>
       <c r="F87" s="3">
         <f t="shared" si="35"/>
-        <v>1.0440000000000003</v>
+        <v>1.3920000000000001</v>
       </c>
       <c r="G87" s="5">
         <v>42559</v>
@@ -6359,16 +6347,18 @@
         <v>0.28799999999999998</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E88" s="3">
         <f t="shared" ref="E88:E90" si="36">C88/D88</f>
-        <v>0.86399999999999999</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="F88" s="3">
         <f t="shared" si="35"/>
-        <v>0.39799999999999996</v>
+        <v>0.53066666666666662</v>
+      </c>
+      <c r="G88" s="5">
+        <v>42562</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -6382,16 +6372,18 @@
         <v>0.11</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E89" s="3">
         <f t="shared" si="36"/>
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="F89" s="3">
         <f t="shared" si="35"/>
-        <v>0.39799999999999996</v>
+        <v>0.53066666666666662</v>
+      </c>
+      <c r="G89" s="5">
+        <v>42562</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -6402,8 +6394,7 @@
         <v>171</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="25"/>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E90" s="3">
         <f t="shared" si="36"/>
@@ -6411,7 +6402,10 @@
       </c>
       <c r="F90" s="3">
         <f t="shared" si="35"/>
-        <v>0.39799999999999996</v>
+        <v>0.53066666666666662</v>
+      </c>
+      <c r="G90" s="5">
+        <v>42562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Log partial experiment, and we'll just hope that Titan manages to save the thing
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -808,6 +808,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="C93" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Grey:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+This one looked like it was gonna be the best of the lot, but the power outage took out the network and I lost the SSH tunnel. So we'll never know.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1500,7 +1522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="180">
   <si>
     <t>Test Group</t>
   </si>
@@ -2151,27 +2173,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2869,11 +2871,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2136460688"/>
-        <c:axId val="-2136456992"/>
+        <c:axId val="2131162656"/>
+        <c:axId val="2131176848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2136460688"/>
+        <c:axId val="2131162656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +2918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136456992"/>
+        <c:crossAx val="2131176848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2924,7 +2926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136456992"/>
+        <c:axId val="2131176848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,7 +2977,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2136460688"/>
+        <c:crossAx val="2131162656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3867,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6327,7 +6329,7 @@
         <v>1.36</v>
       </c>
       <c r="F85" s="3">
-        <f t="shared" ref="F85:F91" si="35">AVERAGEIF(B:B,B85,E:E)</f>
+        <f t="shared" ref="F85:F90" si="35">AVERAGEIF(B:B,B85,E:E)</f>
         <v>1.3920000000000001</v>
       </c>
       <c r="G85" s="5">
@@ -6496,7 +6498,13 @@
       </c>
       <c r="F91" s="3">
         <f t="shared" ref="F91:F93" si="38">AVERAGEIF(B:B,B91,E:E)</f>
-        <v>0.20266666666666666</v>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G91" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -6506,16 +6514,25 @@
       <c r="B92" t="s">
         <v>177</v>
       </c>
+      <c r="C92" s="1">
+        <v>0.216</v>
+      </c>
       <c r="D92" s="1">
         <v>0.25</v>
       </c>
       <c r="E92" s="3">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="F92" s="3">
         <f t="shared" si="38"/>
-        <v>0.20266666666666666</v>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G92" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -6534,19 +6551,25 @@
       </c>
       <c r="F93" s="3">
         <f t="shared" si="38"/>
-        <v>0.20266666666666666</v>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G93" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="15" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="14" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="13" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8624,14 +8647,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8967,20 +8990,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Prep for new experiment
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -852,6 +852,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="B97" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">dFT1:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">A shallower neural network, using FFT data, on 1-second windows.
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1544,7 +1567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="188">
   <si>
     <t>Test Group</t>
   </si>
@@ -2096,6 +2119,18 @@
   </si>
   <si>
     <t>FFT2.0.2</t>
+  </si>
+  <si>
+    <t>dFT1.0.0</t>
+  </si>
+  <si>
+    <t>dFT1</t>
+  </si>
+  <si>
+    <t>dFT1.0.1</t>
+  </si>
+  <si>
+    <t>dFT1.0.2</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2242,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3921,10 +3976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6551,7 +6606,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="F91" s="3">
-        <f t="shared" ref="F91:F96" si="38">AVERAGEIF(B:B,B91,E:E)</f>
+        <f t="shared" ref="F91:F98" si="38">AVERAGEIF(B:B,B91,E:E)</f>
         <v>0.49066666666666664</v>
       </c>
       <c r="G91" s="5">
@@ -6698,16 +6753,73 @@
         <v>78</v>
       </c>
     </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>184</v>
+      </c>
+      <c r="B97" t="s">
+        <v>185</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E97" s="3">
+        <f t="shared" ref="E97:E99" si="40">C97/D97</f>
+        <v>0</v>
+      </c>
+      <c r="F97" s="3">
+        <f t="shared" ref="F97:F99" si="41">AVERAGEIF(B:B,B97,E:E)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>186</v>
+      </c>
+      <c r="B98" t="s">
+        <v>185</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="3">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>187</v>
+      </c>
+      <c r="B99" t="s">
+        <v>185</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E99" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="3">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="15" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="17" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="14" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="13" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="15" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8785,14 +8897,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="11" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="10" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9128,20 +9240,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="5" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finish experiment from yesterday
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -1589,7 +1589,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="194">
   <si>
     <t>Test Group</t>
   </si>
@@ -2168,6 +2168,9 @@
   </si>
   <si>
     <t>SAM1.0.2</t>
+  </si>
+  <si>
+    <t>08.15.txt</t>
   </si>
 </sst>
 </file>
@@ -2279,67 +2282,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3037,11 +2980,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2146591648"/>
-        <c:axId val="2146592064"/>
+        <c:axId val="-2118024896"/>
+        <c:axId val="-2118021296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2146591648"/>
+        <c:axId val="-2118024896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,7 +3027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2146592064"/>
+        <c:crossAx val="-2118021296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3092,7 +3035,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146592064"/>
+        <c:axId val="-2118021296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3143,7 +3086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2146591648"/>
+        <c:crossAx val="-2118024896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4036,7 +3979,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6663,7 +6606,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="F91" s="3">
-        <f t="shared" ref="F91:F98" si="38">AVERAGEIF(B:B,B91,E:E)</f>
+        <f t="shared" ref="F91:F96" si="38">AVERAGEIF(B:B,B91,E:E)</f>
         <v>0.49066666666666664</v>
       </c>
       <c r="G91" s="5">
@@ -6828,7 +6771,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="3">
-        <f t="shared" ref="F97:F100" si="41">AVERAGEIF(B:B,B97,E:E)</f>
+        <f t="shared" ref="F97:F99" si="41">AVERAGEIF(B:B,B97,E:E)</f>
         <v>1.0053333333333334</v>
       </c>
       <c r="G97" s="5">
@@ -6901,16 +6844,25 @@
       <c r="B100" t="s">
         <v>189</v>
       </c>
+      <c r="C100" s="1">
+        <v>0.35599999999999998</v>
+      </c>
       <c r="D100" s="1">
         <v>0.25</v>
       </c>
       <c r="E100" s="3">
         <f t="shared" ref="E100:E102" si="42">C100/D100</f>
-        <v>0</v>
+        <v>1.4239999999999999</v>
       </c>
       <c r="F100" s="3">
         <f t="shared" ref="F100:F102" si="43">AVERAGEIF(B:B,B100,E:E)</f>
-        <v>0</v>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G100" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -6920,16 +6872,25 @@
       <c r="B101" t="s">
         <v>189</v>
       </c>
+      <c r="C101" s="1">
+        <v>0.45</v>
+      </c>
       <c r="D101" s="1">
         <v>0.25</v>
       </c>
       <c r="E101" s="3">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="F101" s="3">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G101" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -6939,28 +6900,37 @@
       <c r="B102" t="s">
         <v>189</v>
       </c>
+      <c r="C102" s="1">
+        <v>0.38600000000000001</v>
+      </c>
       <c r="D102" s="1">
         <v>0.25</v>
       </c>
       <c r="E102" s="3">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1.544</v>
       </c>
       <c r="F102" s="3">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G102" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="19" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="18" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="17" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9038,14 +9008,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="15" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="14" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="13" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9381,20 +9351,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="11" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="10" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="9" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More charts, and using them.
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
-    <sheet name="GenreID" sheetId="3" r:id="rId2"/>
-    <sheet name="15-Series" sheetId="2" r:id="rId3"/>
+    <sheet name="InstrumentID" sheetId="4" r:id="rId2"/>
+    <sheet name="GenreID" sheetId="3" r:id="rId3"/>
+    <sheet name="15-Series" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -938,17 +939,17 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Midpoint 3</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Feeds raw samples from :30-:40 into NN, attempting to map the song into one of three genres: art, pop, or traditional.
+          <t xml:space="preserve">INS4Titan:
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>The 4th in a series of non-logged experiments, training for instrument identification on windows. Named because this one was run on Titan.
+Note: as this run doesn't have evaluation code implemented, the logged accuracy is the final validation accuracy reported by the training phase.</t>
         </r>
       </text>
     </comment>
@@ -961,16 +962,17 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Midpoint 3
+          <t>Instrument5:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Instrument identification still, using a larger neural network.
 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Feeds raw samples from :00-:10 into NN, attempting to map the song into one of three genres: art, pop, or traditional.</t>
         </r>
       </text>
     </comment>
@@ -983,16 +985,16 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>StartDouble3</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Reads from :00 to :20, feeds raw samples into the neural network, and then attempts to categorize them into three genres: art, pop, or traditional.</t>
+          <t xml:space="preserve">Instrument6:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Looking at different neural network shapes for the Instrument series.</t>
         </r>
       </text>
     </comment>
@@ -1000,13 +1002,21 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">NewShape3
-Testing the same thing as StartDouble3, but with the initial layer of the NN widened out to 2* size.
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Instrument7:
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>More tweaks of neural network shape. This one is a series of layers of decreasing powers of two neurons.</t>
         </r>
       </text>
     </comment>
@@ -1019,7 +1029,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">DeeperNN
+          <t xml:space="preserve">Instrument8:
 </t>
         </r>
         <r>
@@ -1028,7 +1038,25 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Testing the same thing as NewShape3, but with an additional 64-neuron, tanh layer.</t>
+          <t xml:space="preserve">Testing the Instrument series using the same network shape as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Instrument7</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">, but with an input window of twice the size.
+</t>
         </r>
       </text>
     </comment>
@@ -1041,7 +1069,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">MidpointWide
+          <t xml:space="preserve">Instrument9:
 </t>
         </r>
         <r>
@@ -1050,8 +1078,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Testing the same thing as NewShape3, but using the :10-:30 chunk instead of :00-:20
-</t>
+          <t>No changes from Instrument8, just using a more filled-out dataset.</t>
         </r>
       </text>
     </comment>
@@ -1064,35 +1091,16 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>15.Start</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Part of the </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>15.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> meta-group.
-Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+          <t xml:space="preserve">SAM1:
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Longer input samples, hopefully more overlap assuming I tweaked that right, and back to feeeding raw samples rather than FFT data.</t>
         </r>
       </text>
     </comment>
@@ -1105,18 +1113,16 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>15.Minute</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Part of the 15. meta-group.
-Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+          <t xml:space="preserve">SAM2:
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>One tweak since SAM1: using 3 seconds instead of 2.</t>
         </r>
       </text>
     </comment>
@@ -1129,7 +1135,29 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>15.Mix</t>
+          <t xml:space="preserve">FFT1:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Using the same neural network setup and input as Instrument9, but the input is being fed through an FFT before going into the neural network.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Grey:</t>
         </r>
         <r>
           <rPr>
@@ -1138,9 +1166,7 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-Part of the 15. meta-group.
-Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
-</t>
+This one looked like it was gonna be the best of the lot, but the power outage took out the network and I lost the SSH tunnel. So we'll never know.</t>
         </r>
       </text>
     </comment>
@@ -1153,7 +1179,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Lessen_Dropout
+          <t xml:space="preserve">FFT2:
 </t>
         </r>
         <r>
@@ -1162,7 +1188,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Testing the normal neural network layout with the 'dropout' setting dropped from 0.5 to 0.25</t>
+          <t>No changes since FFT1, but hopefully we can get through this one without a power failure.</t>
         </r>
       </text>
     </comment>
@@ -1175,7 +1201,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">15.Mix.exNULL
+          <t xml:space="preserve">dFT1:
 </t>
         </r>
         <r>
@@ -1184,326 +1210,8 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Data loss problem with this one - I'm leaving the record in here, but culling it from the rest of the 15.Mix.extended series.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B33" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">15.Mix.extended
+          <t xml:space="preserve">A shallower neural network, using FFT data, on 1-second windows.
 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>A trial of the 15.Mix using a batch size larger than the dataset - rolling over the end of the dataset will force rebuilding of some songs, which will allow us to artificially incrase the size of the dataset by a large amount.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B38" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">MTRN1:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Multiple trainings on the same neural network.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B44" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">default:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Create a default set of weights and a model for testing to see which songs are mis-identified every time.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B47" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>newCategories:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Using the data from the </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>default</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> test, I shuffled around some of the ways that genres were mapped to meta-genres. Testing the results here.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B50" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">newDataSet:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">Testing the same thing as </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>newCategories</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>, utilizing an updated data set that includes more music in the 'art' meta-genre.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B53" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>newDataSet.1:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Secondary training on the networks produced by </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>newDataSet</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A56" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">Unhandled exception in the </t>
-        </r>
-        <r>
-          <rPr>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>next_batch</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> code crashed the run after the first one - spent a while fixing it.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B56" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">20Sec1Minute:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Feeds in samples 20 seconds long, non-randomized, starting 1 minute into the song.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B60" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">BiggerNN:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Using a significantly-larger neural network with the 20-seconds-at-1-minute input - added another layer, and gave it a pyramid shape, so 256-128-64-end.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B63" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">The120:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Limiting the amount of songs being fed in in an effort to reduce the amount of overfitting.
-Which, with only 120 samples, probably won't work. Dang.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B66" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">The120Repeat:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">Use the samples from </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>The120</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>, but set to randomize and run through them all multiple times.</t>
         </r>
       </text>
     </comment>
@@ -1526,6 +1234,594 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t>Midpoint 3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Feeds raw samples from :30-:40 into NN, attempting to map the song into one of three genres: art, pop, or traditional.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Midpoint 3
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Feeds raw samples from :00-:10 into NN, attempting to map the song into one of three genres: art, pop, or traditional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>StartDouble3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Reads from :00 to :20, feeds raw samples into the neural network, and then attempts to categorize them into three genres: art, pop, or traditional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">NewShape3
+Testing the same thing as StartDouble3, but with the initial layer of the NN widened out to 2* size.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">DeeperNN
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Testing the same thing as NewShape3, but with an additional 64-neuron, tanh layer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">MidpointWide
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Testing the same thing as NewShape3, but using the :10-:30 chunk instead of :00-:20
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Start</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> meta-group.
+Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Minute</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Mix</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Lessen_Dropout
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Testing the normal neural network layout with the 'dropout' setting dropped from 0.5 to 0.25</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">15.Mix.exNULL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Data loss problem with this one - I'm leaving the record in here, but culling it from the rest of the 15.Mix.extended series.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">15.Mix.extended
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>A trial of the 15.Mix using a batch size larger than the dataset - rolling over the end of the dataset will force rebuilding of some songs, which will allow us to artificially incrase the size of the dataset by a large amount.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">MTRN1:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Multiple trainings on the same neural network.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">default:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Create a default set of weights and a model for testing to see which songs are mis-identified every time.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newCategories:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Using the data from the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>default</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> test, I shuffled around some of the ways that genres were mapped to meta-genres. Testing the results here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">newDataSet:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Testing the same thing as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newCategories</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>, utilizing an updated data set that includes more music in the 'art' meta-genre.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B53" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newDataSet.1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Secondary training on the networks produced by </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>newDataSet</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Unhandled exception in the </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>next_batch</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> code crashed the run after the first one - spent a while fixing it.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">20Sec1Minute:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Feeds in samples 20 seconds long, non-randomized, starting 1 minute into the song.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B60" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">BiggerNN:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Using a significantly-larger neural network with the 20-seconds-at-1-minute input - added another layer, and gave it a pyramid shape, so 256-128-64-end.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B63" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">The120:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Limiting the amount of songs being fed in in an effort to reduce the amount of overfitting.
+Which, with only 120 samples, probably won't work. Dang.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">The120Repeat:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Use the samples from </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>The120</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>, but set to randomize and run through them all multiple times.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Grey</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t>15.Start</t>
         </r>
         <r>
@@ -1611,7 +1907,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="199">
   <si>
     <t>Test Group</t>
   </si>
@@ -2301,7 +2597,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2310,6 +2606,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -2319,7 +2617,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2484,8 +2782,59 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF729FCF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2495,6 +2844,464 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>InstrumentID!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>InstrumentID!$B$2:$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>INS4Titan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>INS4Titan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INS4Titan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Instrument5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Instrument5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Instrument5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Instrument6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Instrument6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Instrument6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Instrument7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Instrument7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Instrument7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Instrument8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Instrument8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Instrument8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Instrument9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Instrument9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Instrument9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>SAM1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SAM1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>SAM1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>SAM2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>SAM2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>SAM2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>FFT1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>FFT1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>FFT1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>FFT2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>FFT2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>FFT2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>dFT1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>dFT1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>dFT1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>InstrumentID!$C$2:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.324</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.382</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.368</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.376</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.338</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.354</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.288</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.264</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.356</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.386</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.218</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.166</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.176</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.216</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.236</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.268</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.472</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.252</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2126525040"/>
+        <c:axId val="2126528128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2126525040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126528128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2126528128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2126525040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2561,7 +3368,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="729FCF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3017,11 +3824,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2137040656"/>
-        <c:axId val="2137030384"/>
+        <c:axId val="2122228640"/>
+        <c:axId val="2122232320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137040656"/>
+        <c:axId val="2122228640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3064,7 +3871,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137030384"/>
+        <c:crossAx val="2122232320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3072,7 +3879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137030384"/>
+        <c:axId val="2122232320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3123,7 +3930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137040656"/>
+        <c:crossAx val="2122228640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3173,6 +3980,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3715,7 +4562,545 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>711198</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4015,8 +5400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7044,6 +8429,997 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="top10" dxfId="17" priority="4" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="16" priority="3" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="top10" dxfId="15" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D4" si="0">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E25" si="1">C2/D2</f>
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ref="F2:F34" si="2">AVERAGEIF(B:B,B2,E:E)</f>
+        <v>1.024</v>
+      </c>
+      <c r="G2" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.97200000000000009</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="2"/>
+        <v>1.024</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.37</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>1.024</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.528</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4586666666666666</v>
+      </c>
+      <c r="G5" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3759999999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4586666666666666</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>1.472</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4586666666666666</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42557</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>1.208</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2826666666666666</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3759999999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2826666666666666</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.316</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>1.264</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2826666666666666</v>
+      </c>
+      <c r="G10" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.376</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>1.504</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4186666666666667</v>
+      </c>
+      <c r="G11" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3520000000000001</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4186666666666667</v>
+      </c>
+      <c r="G12" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4186666666666667</v>
+      </c>
+      <c r="G13" s="5">
+        <v>42558</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.34</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>1.36</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3920000000000001</v>
+      </c>
+      <c r="G14" s="5">
+        <v>42559</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3920000000000001</v>
+      </c>
+      <c r="G15" s="5">
+        <v>42559</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4159999999999999</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3920000000000001</v>
+      </c>
+      <c r="G16" s="5">
+        <v>42559</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1519999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8826666666666666</v>
+      </c>
+      <c r="G17" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.44</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8826666666666666</v>
+      </c>
+      <c r="G18" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>1.056</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8826666666666666</v>
+      </c>
+      <c r="G19" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4239999999999999</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G20" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G21" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>1.544</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5893333333333335</v>
+      </c>
+      <c r="G22" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.218</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.872</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="G23" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="1"/>
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="G24" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="1"/>
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="G25" s="5">
+        <v>42564</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.152</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" ref="E26:E34" si="3">C26/D26</f>
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G26" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.216</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="3"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G27" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="G28" s="5">
+        <v>42562</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="3"/>
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3013333333333332</v>
+      </c>
+      <c r="G29" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3013333333333332</v>
+      </c>
+      <c r="G30" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B31" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="3"/>
+        <v>1.8879999999999999</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3013333333333332</v>
+      </c>
+      <c r="G31" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0053333333333334</v>
+      </c>
+      <c r="G32" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.252</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0053333333333334</v>
+      </c>
+      <c r="G33" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.252</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="3"/>
+        <v>1.008</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0053333333333334</v>
+      </c>
+      <c r="G34" s="5">
+        <v>42563</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
@@ -7056,17 +9432,17 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9146,7 +11522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update log files with the new graphs I made in a sandbox
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Documents/More/Bitbucket/nAud/logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
     <sheet name="InstrumentID" sheetId="4" r:id="rId2"/>
     <sheet name="GenreID" sheetId="3" r:id="rId3"/>
-    <sheet name="15-Series" sheetId="2" r:id="rId4"/>
+    <sheet name="15.comparison" sheetId="5" r:id="rId4"/>
+    <sheet name="15-Series" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -1813,6 +1814,105 @@
     <author>Grey</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Start</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> meta-group.
+Tests the first 15 seconds of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Minute</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests the 15 seconds from 1:00 to 1:15 of the sample against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>15.Mix</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Part of the 15. meta-group.
+Tests a composite 15 seconds (made up of 3 5-second chunks taken from random points within the sample) against a specific neural network form. The other meta-group members test different parts of the song.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Grey</author>
+  </authors>
+  <commentList>
     <comment ref="B2" authorId="0">
       <text>
         <r>
@@ -1907,7 +2007,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="205">
   <si>
     <t>Test Group</t>
   </si>
@@ -2504,6 +2604,24 @@
   </si>
   <si>
     <t>run.txt</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>1 Minute</t>
+  </si>
+  <si>
+    <t>Shuffle</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2735,541 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3145,11 +3797,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2126525040"/>
-        <c:axId val="2126528128"/>
+        <c:axId val="2121515440"/>
+        <c:axId val="2121518880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126525040"/>
+        <c:axId val="2121515440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3192,7 +3844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126528128"/>
+        <c:crossAx val="2121518880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3200,7 +3852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126528128"/>
+        <c:axId val="2121518880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3252,7 +3904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126525040"/>
+        <c:crossAx val="2121515440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3316,6 +3968,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3824,11 +4477,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2122228640"/>
-        <c:axId val="2122232320"/>
+        <c:axId val="2113059456"/>
+        <c:axId val="2113055760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2122228640"/>
+        <c:axId val="2113059456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3871,7 +4524,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122232320"/>
+        <c:crossAx val="2113055760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3879,7 +4532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122232320"/>
+        <c:axId val="2113055760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3930,7 +4583,433 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2122228640"/>
+        <c:crossAx val="2113059456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Accuracy of Tests at Varying</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> Sample Locations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$14:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$C$14:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.7265625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72265625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$14:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$D$14:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.74609375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73828125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70703125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$E$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$14:$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$E$14:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.76953125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7734375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2037146144"/>
+        <c:axId val="-2147218656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2037146144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2147218656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2147218656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2037146144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4020,6 +5099,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5065,20 +6184,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>711198</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>622298</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5104,20 +6726,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>395817</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>268817</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>332317</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>205317</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>235701</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5400,8 +7057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8429,14 +10086,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="17" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="59" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="16" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="58" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="15" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="57" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8450,8 +10107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9420,14 +11077,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="13" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="55" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="12" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="54" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="53" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9442,7 +11099,8 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11505,14 +13163,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="9" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="51" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="8" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="50" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="49" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11523,6 +13181,401 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.7265625</v>
+      </c>
+      <c r="D1" s="1">
+        <f t="shared" ref="D1:D9" si="0">1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E1" s="3">
+        <f t="shared" ref="E1:E9" si="1">C1/D1</f>
+        <v>2.1796875</v>
+      </c>
+      <c r="F1" s="3">
+        <f t="shared" ref="F1:F9" si="2">AVERAGEIF(B:B,B1,E:E)</f>
+        <v>2.2421875</v>
+      </c>
+      <c r="G1" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" si="1"/>
+        <v>2.23828125</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2421875</v>
+      </c>
+      <c r="G2" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.76953125</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="1"/>
+        <v>2.30859375</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" si="2"/>
+        <v>2.2421875</v>
+      </c>
+      <c r="G3" s="6">
+        <v>42538</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.72265625</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.16796875</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.73828125</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>2.21484375</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G5" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.7734375</v>
+      </c>
+      <c r="D6" s="1">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3203125</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>2.234375</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.70703125</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>2.12109375</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>2.4375</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>2.33203125</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42538</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.7265625</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.74609375</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.76953125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.72265625</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.73828125</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.7734375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.70703125</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E9">
+    <cfRule type="top10" dxfId="41" priority="20" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F9">
+    <cfRule type="top10" dxfId="39" priority="19" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="top10" dxfId="37" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="36" priority="18" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="top10" dxfId="33" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="top10" dxfId="29" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="top10" dxfId="25" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="top10" dxfId="21" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="top10" dxfId="17" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="top10" dxfId="13" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="top10" dxfId="9" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:E17">
+    <cfRule type="top10" dxfId="5" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -11848,20 +13901,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="5" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="47" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="4" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="46" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="3" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="45" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="1" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="43" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
always with the updating of graphs
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -1217,28 +1217,6 @@
       </text>
     </comment>
     <comment ref="M37" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Grey:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-This one looked like it was gonna be the best of the lot, but the power outage took out the network and I lost the SSH tunnel. So we'll never know.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M55" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3931,11 +3909,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2098512592"/>
-        <c:axId val="-2098509120"/>
+        <c:axId val="2124201360"/>
+        <c:axId val="2124204848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098512592"/>
+        <c:axId val="2124201360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3978,7 +3956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098509120"/>
+        <c:crossAx val="2124204848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3986,7 +3964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098509120"/>
+        <c:axId val="2124204848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4038,7 +4016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098512592"/>
+        <c:crossAx val="2124201360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4449,11 +4427,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2098442128"/>
-        <c:axId val="-2098438640"/>
+        <c:axId val="2124263184"/>
+        <c:axId val="2124266672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098442128"/>
+        <c:axId val="2124263184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4496,7 +4474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098438640"/>
+        <c:crossAx val="2124266672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4504,7 +4482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098438640"/>
+        <c:axId val="2124266672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4555,7 +4533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098442128"/>
+        <c:crossAx val="2124263184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4664,13 +4642,17 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="5000"/>
+              <a:rPr lang="en-US" sz="5000">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
               <a:t>Accuracy of FFT vs. Sample Input</a:t>
             </a:r>
           </a:p>
@@ -4697,9 +4679,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -4754,9 +4736,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.152</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.382</c:v>
                 </c:pt>
@@ -4805,9 +4784,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.216</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.344</c:v>
                 </c:pt>
@@ -4856,9 +4832,6 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.368</c:v>
                 </c:pt>
@@ -4908,7 +4881,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.236</c:v>
+                  <c:v>0.152</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.302</c:v>
@@ -4959,7 +4932,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.268</c:v>
+                  <c:v>0.216</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.344</c:v>
@@ -5010,7 +4983,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.472</c:v>
+                  <c:v>0.236</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.316</c:v>
@@ -5061,7 +5034,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.268</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.376</c:v>
@@ -5112,7 +5085,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>0.472</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.338</c:v>
@@ -5213,6 +5186,9 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.34</c:v>
                 </c:pt>
@@ -5261,6 +5237,9 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0.35</c:v>
                 </c:pt>
@@ -5470,11 +5449,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2092528288"/>
-        <c:axId val="-2092531712"/>
+        <c:axId val="2096057520"/>
+        <c:axId val="2124231344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2092528288"/>
+        <c:axId val="2096057520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5509,15 +5488,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092531712"/>
+        <c:crossAx val="2124231344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5525,7 +5504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2092531712"/>
+        <c:axId val="2124231344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5554,15 +5533,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092528288"/>
+        <c:crossAx val="2096057520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6135,11 +6114,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2108945600"/>
-        <c:axId val="-2108938240"/>
+        <c:axId val="2095932048"/>
+        <c:axId val="2095965456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108945600"/>
+        <c:axId val="2095932048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +6161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108938240"/>
+        <c:crossAx val="2095965456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6190,7 +6169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108938240"/>
+        <c:axId val="2095965456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6241,7 +6220,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2108945600"/>
+        <c:crossAx val="2095932048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6311,27 +6290,39 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="5000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="4400"/>
+              <a:rPr lang="en-US" sz="4000">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
               <a:t>Accuracy of Tests at Varying</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="4400" baseline="0"/>
+              <a:rPr lang="en-US" sz="4000" baseline="0">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
               <a:t> Sample Locations</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="4400"/>
+            <a:endParaRPr lang="en-US" sz="4000">
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6349,16 +6340,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="5000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -6396,6 +6387,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'15.comparison'!$B$14:$B$16</c:f>
@@ -6456,6 +6506,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'15.comparison'!$B$14:$B$16</c:f>
@@ -6516,6 +6625,65 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'15.comparison'!$B$14:$B$16</c:f>
@@ -6562,11 +6730,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2098367088"/>
-        <c:axId val="-2098363616"/>
+        <c:axId val="2124325440"/>
+        <c:axId val="2124328912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2098367088"/>
+        <c:axId val="2124325440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6601,15 +6769,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098363616"/>
+        <c:crossAx val="2124328912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6617,7 +6785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098363616"/>
+        <c:axId val="2124328912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6646,15 +6814,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098367088"/>
+        <c:crossAx val="2124325440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9482,16 +9650,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>393699</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>629556</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>192315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>33866</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>269723</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>68943</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12898,8 +13066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView topLeftCell="K35" workbookViewId="0">
-      <selection activeCell="Z42" sqref="Z42"/>
+    <sheetView tabSelected="1" topLeftCell="T43" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14017,31 +14185,28 @@
       <c r="J55" t="s">
         <v>205</v>
       </c>
-      <c r="K55" s="9">
+      <c r="N55" s="9">
         <v>0.152</v>
       </c>
-      <c r="L55" s="9">
+      <c r="O55" s="9">
         <v>0.216</v>
       </c>
-      <c r="M55" s="9">
-        <v>0</v>
-      </c>
-      <c r="N55" s="9">
+      <c r="P55" s="9">
         <v>0.23599999999999999</v>
       </c>
-      <c r="O55" s="9">
+      <c r="Q55" s="9">
         <v>0.26800000000000002</v>
       </c>
-      <c r="P55" s="9">
+      <c r="R55" s="9">
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q55" s="9">
+      <c r="S55" s="9">
         <v>0.25</v>
       </c>
-      <c r="R55" s="9">
+      <c r="T55" s="9">
         <v>0.25</v>
       </c>
-      <c r="S55" s="9">
+      <c r="U55" s="9">
         <v>0.25</v>
       </c>
     </row>
@@ -14150,13 +14315,13 @@
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55:M55">
+  <conditionalFormatting sqref="N55:O55">
     <cfRule type="top10" dxfId="43" priority="13" percent="1" rank="10"/>
     <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N55:P55">
+  <conditionalFormatting sqref="P55:R55">
     <cfRule type="top10" dxfId="41" priority="11" percent="1" rank="10"/>
     <cfRule type="cellIs" dxfId="40" priority="12" operator="greaterThan">
       <formula>95</formula>
@@ -16288,8 +16453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change 'shuffle' in graph to 'random points'
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Documents/More/Bitbucket/nAud/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -2634,9 +2634,6 @@
     <t>1 Minute</t>
   </si>
   <si>
-    <t>Shuffle</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
@@ -2650,6 +2647,9 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>Random Selection</t>
   </si>
 </sst>
 </file>
@@ -3909,11 +3909,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2124201360"/>
-        <c:axId val="2124204848"/>
+        <c:axId val="-2114652240"/>
+        <c:axId val="-2114655840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124201360"/>
+        <c:axId val="-2114652240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3956,7 +3956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124204848"/>
+        <c:crossAx val="-2114655840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3964,7 +3964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124204848"/>
+        <c:axId val="-2114655840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4016,7 +4016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124201360"/>
+        <c:crossAx val="-2114652240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4427,11 +4427,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2124263184"/>
-        <c:axId val="2124266672"/>
+        <c:axId val="-2113487840"/>
+        <c:axId val="-2113484352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124263184"/>
+        <c:axId val="-2113487840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4474,7 +4474,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124266672"/>
+        <c:crossAx val="-2113484352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4482,7 +4482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124266672"/>
+        <c:axId val="-2113484352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4533,7 +4533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124263184"/>
+        <c:crossAx val="-2113487840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5449,11 +5449,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2096057520"/>
-        <c:axId val="2124231344"/>
+        <c:axId val="-2113419648"/>
+        <c:axId val="-2113416224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2096057520"/>
+        <c:axId val="-2113419648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5496,7 +5496,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124231344"/>
+        <c:crossAx val="-2113416224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5504,7 +5504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124231344"/>
+        <c:axId val="-2113416224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5541,7 +5541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096057520"/>
+        <c:crossAx val="-2113419648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5605,7 +5605,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6114,11 +6113,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2095932048"/>
-        <c:axId val="2095965456"/>
+        <c:axId val="-2114686496"/>
+        <c:axId val="-2114682288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095932048"/>
+        <c:axId val="-2114686496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6161,7 +6160,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095965456"/>
+        <c:crossAx val="-2114682288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6169,7 +6168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095965456"/>
+        <c:axId val="-2114682288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6220,7 +6219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095932048"/>
+        <c:crossAx val="-2114686496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6458,7 +6457,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Shuffle</c:v>
+                  <c:v>Random Selection</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6577,7 +6576,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Shuffle</c:v>
+                  <c:v>Random Selection</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6696,7 +6695,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Shuffle</c:v>
+                  <c:v>Random Selection</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6730,11 +6729,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2124325440"/>
-        <c:axId val="2124328912"/>
+        <c:axId val="-2114810304"/>
+        <c:axId val="-2114813856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124325440"/>
+        <c:axId val="-2114810304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6777,7 +6776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124328912"/>
+        <c:crossAx val="-2114813856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6785,7 +6784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124328912"/>
+        <c:axId val="-2114813856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6822,7 +6821,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2124325440"/>
+        <c:crossAx val="-2114810304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13066,7 +13065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T43" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView topLeftCell="T43" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="AB47" sqref="AB47"/>
     </sheetView>
   </sheetViews>
@@ -14036,18 +14035,18 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K36" t="s">
+        <v>201</v>
+      </c>
+      <c r="L36" t="s">
         <v>202</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>203</v>
-      </c>
-      <c r="M36" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J37" t="s">
         <v>177</v>
@@ -14064,7 +14063,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J38" t="s">
         <v>180</v>
@@ -14081,7 +14080,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J39" t="s">
         <v>185</v>
@@ -14098,7 +14097,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J40" t="s">
         <v>151</v>
@@ -14115,7 +14114,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J41" t="s">
         <v>156</v>
@@ -14132,7 +14131,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J42" t="s">
         <v>161</v>
@@ -14149,7 +14148,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J43" t="s">
         <v>167</v>
@@ -14166,7 +14165,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J44" t="s">
         <v>171</v>
@@ -14183,7 +14182,7 @@
     </row>
     <row r="55" spans="10:25" x14ac:dyDescent="0.2">
       <c r="J55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N55" s="9">
         <v>0.152</v>
@@ -14212,7 +14211,7 @@
     </row>
     <row r="56" spans="10:25" x14ac:dyDescent="0.2">
       <c r="J56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K56" s="9">
         <v>0.38200000000000001</v>
@@ -16453,8 +16452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16722,13 +16721,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" t="s">
         <v>202</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>203</v>
-      </c>
-      <c r="E13" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -16761,7 +16760,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C16" s="1">
         <v>0.8125</v>

</xml_diff>

<commit_message>
but this time WITHOUT the typo
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -2649,7 +2649,7 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Random Selection</t>
+    <t>Random Points</t>
   </si>
 </sst>
 </file>
@@ -3909,11 +3909,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2114652240"/>
-        <c:axId val="-2114655840"/>
+        <c:axId val="2146014560"/>
+        <c:axId val="2146018016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114652240"/>
+        <c:axId val="2146014560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3956,7 +3956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114655840"/>
+        <c:crossAx val="2146018016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3964,7 +3964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114655840"/>
+        <c:axId val="2146018016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4016,7 +4016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114652240"/>
+        <c:crossAx val="2146014560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4110,7 +4110,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4427,11 +4426,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2113487840"/>
-        <c:axId val="-2113484352"/>
+        <c:axId val="2146168432"/>
+        <c:axId val="2146171920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113487840"/>
+        <c:axId val="2146168432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4474,7 +4473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113484352"/>
+        <c:crossAx val="2146171920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4482,7 +4481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113484352"/>
+        <c:axId val="2146171920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4533,7 +4532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113487840"/>
+        <c:crossAx val="2146168432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4547,7 +4546,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4658,7 +4656,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5449,11 +5446,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2113419648"/>
-        <c:axId val="-2113416224"/>
+        <c:axId val="2146293792"/>
+        <c:axId val="2146297216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2113419648"/>
+        <c:axId val="2146293792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5496,7 +5493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113416224"/>
+        <c:crossAx val="2146297216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5504,7 +5501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2113416224"/>
+        <c:axId val="2146297216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5541,7 +5538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113419648"/>
+        <c:crossAx val="2146293792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6113,11 +6110,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2114686496"/>
-        <c:axId val="-2114682288"/>
+        <c:axId val="2112476496"/>
+        <c:axId val="2112460592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114686496"/>
+        <c:axId val="2112476496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6160,7 +6157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114682288"/>
+        <c:crossAx val="2112460592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6168,7 +6165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114682288"/>
+        <c:axId val="2112460592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6219,7 +6216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114686496"/>
+        <c:crossAx val="2112476496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6457,7 +6454,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Random Selection</c:v>
+                  <c:v>Random Points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6576,7 +6573,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Random Selection</c:v>
+                  <c:v>Random Points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6695,7 +6692,7 @@
                   <c:v>1 Minute</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Random Selection</c:v>
+                  <c:v>Random Points</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6729,11 +6726,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2114810304"/>
-        <c:axId val="-2114813856"/>
+        <c:axId val="2112231392"/>
+        <c:axId val="2112230064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114810304"/>
+        <c:axId val="2112231392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6776,7 +6773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114813856"/>
+        <c:crossAx val="2112230064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6784,7 +6781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114813856"/>
+        <c:axId val="2112230064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6821,7 +6818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114810304"/>
+        <c:crossAx val="2112231392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16452,7 +16449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Log experiment, prep for next one
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -2051,7 +2051,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="221">
   <si>
     <t>Test Group</t>
   </si>
@@ -2711,6 +2711,9 @@
   </si>
   <si>
     <t>08.47.txt</t>
+  </si>
+  <si>
+    <t>08.54.txt</t>
   </si>
 </sst>
 </file>
@@ -10114,7 +10117,7 @@
   <dimension ref="A1:I114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13231,19 +13234,25 @@
       <c r="B109" t="s">
         <v>211</v>
       </c>
+      <c r="C109" s="1">
+        <v>0.51724139164233995</v>
+      </c>
       <c r="D109" s="1">
         <v>0.33</v>
       </c>
       <c r="E109" s="3">
         <f t="shared" ref="E109:E114" si="46">C109/D109</f>
-        <v>0</v>
+        <v>1.5673981564919393</v>
       </c>
       <c r="F109" s="3">
         <f t="shared" ref="F109:F114" si="47">AVERAGEIF(B:B,B109,E:E)</f>
-        <v>0</v>
+        <v>0.97701150986311802</v>
       </c>
       <c r="G109" s="5">
         <v>42572</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -13253,19 +13262,25 @@
       <c r="B110" t="s">
         <v>211</v>
       </c>
+      <c r="C110" s="1">
+        <v>0.20000000099341</v>
+      </c>
       <c r="D110" s="1">
         <v>0.33</v>
       </c>
       <c r="E110" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>0.60606060907093939</v>
       </c>
       <c r="F110" s="3">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>0.97701150986311802</v>
       </c>
       <c r="G110" s="5">
         <v>42572</v>
+      </c>
+      <c r="H110" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -13275,19 +13290,25 @@
       <c r="B111" t="s">
         <v>211</v>
       </c>
+      <c r="C111" s="1">
+        <v>0.25000000212873702</v>
+      </c>
       <c r="D111" s="1">
         <v>0.33</v>
       </c>
       <c r="E111" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>0.75757576402647575</v>
       </c>
       <c r="F111" s="3">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>0.97701150986311802</v>
       </c>
       <c r="G111" s="5">
         <v>42572</v>
+      </c>
+      <c r="H111" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
just keep logging, just keep logging
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -943,6 +943,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="B115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">120g.start, 120g.minute, 120g.mix: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>The same test as above, but using a generator feed rather than a cache, which allows for more mixing throughout, when applicable.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2051,7 +2072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="233">
   <si>
     <t>Test Group</t>
   </si>
@@ -2714,6 +2735,42 @@
   </si>
   <si>
     <t>08.54.txt</t>
+  </si>
+  <si>
+    <t>120g.start</t>
+  </si>
+  <si>
+    <t>120g.minute</t>
+  </si>
+  <si>
+    <t>120g.mix</t>
+  </si>
+  <si>
+    <t>12gS.0.0</t>
+  </si>
+  <si>
+    <t>12gS.0.1</t>
+  </si>
+  <si>
+    <t>12gS.0.2</t>
+  </si>
+  <si>
+    <t>12gM.0.0</t>
+  </si>
+  <si>
+    <t>12gM.0.1</t>
+  </si>
+  <si>
+    <t>12gM.0.2</t>
+  </si>
+  <si>
+    <t>12gX.0.0</t>
+  </si>
+  <si>
+    <t>12gX.0.1</t>
+  </si>
+  <si>
+    <t>12gX.0.2</t>
   </si>
 </sst>
 </file>
@@ -2827,7 +2884,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -10114,10 +10191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13245,7 +13322,7 @@
         <v>1.5673981564919393</v>
       </c>
       <c r="F109" s="3">
-        <f t="shared" ref="F109:F114" si="47">AVERAGEIF(B:B,B109,E:E)</f>
+        <f t="shared" ref="F109:F115" si="47">AVERAGEIF(B:B,B109,E:E)</f>
         <v>0.97701150986311802</v>
       </c>
       <c r="G109" s="5">
@@ -13318,16 +13395,19 @@
       <c r="B112" t="s">
         <v>212</v>
       </c>
+      <c r="C112" s="1">
+        <v>0.23333333929379699</v>
+      </c>
       <c r="D112" s="1">
         <v>0.33</v>
       </c>
       <c r="E112" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>0.70707072513271807</v>
       </c>
       <c r="F112" s="3">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>0.60606061408816669</v>
       </c>
       <c r="G112" s="5">
         <v>42572</v>
@@ -13340,16 +13420,19 @@
       <c r="B113" t="s">
         <v>212</v>
       </c>
+      <c r="C113" s="1">
+        <v>0.36666666865348801</v>
+      </c>
       <c r="D113" s="1">
         <v>0.33</v>
       </c>
       <c r="E113" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1.1111111171317818</v>
       </c>
       <c r="F113" s="3">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>0.60606061408816669</v>
       </c>
       <c r="G113" s="5">
         <v>42572</v>
@@ -13371,22 +13454,220 @@
       </c>
       <c r="F114" s="3">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>0.60606061408816669</v>
       </c>
       <c r="G114" s="5">
         <v>42572</v>
       </c>
     </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>224</v>
+      </c>
+      <c r="B115" t="s">
+        <v>221</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E115" s="3">
+        <f t="shared" ref="E115:E123" si="48">C115/D115</f>
+        <v>0</v>
+      </c>
+      <c r="F115" s="3">
+        <f t="shared" ref="F115:F123" si="49">AVERAGEIF(B:B,B115,E:E)</f>
+        <v>0</v>
+      </c>
+      <c r="G115" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" t="s">
+        <v>221</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E116" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F116" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>226</v>
+      </c>
+      <c r="B117" t="s">
+        <v>221</v>
+      </c>
+      <c r="D117" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E117" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F117" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>227</v>
+      </c>
+      <c r="B118" t="s">
+        <v>222</v>
+      </c>
+      <c r="D118" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E118" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>228</v>
+      </c>
+      <c r="B119" t="s">
+        <v>222</v>
+      </c>
+      <c r="D119" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E119" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F119" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G119" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>229</v>
+      </c>
+      <c r="B120" t="s">
+        <v>222</v>
+      </c>
+      <c r="D120" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E120" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F120" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G120" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>230</v>
+      </c>
+      <c r="B121" t="s">
+        <v>223</v>
+      </c>
+      <c r="D121" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E121" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F121" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>231</v>
+      </c>
+      <c r="B122" t="s">
+        <v>223</v>
+      </c>
+      <c r="D122" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E122" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F122" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="5">
+        <v>42572</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>232</v>
+      </c>
+      <c r="B123" t="s">
+        <v>223</v>
+      </c>
+      <c r="D123" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E123" s="3">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="F123" s="3">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="G123" s="5">
+        <v>42572</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="69" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="68" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="67" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="69" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="68" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14596,98 +14877,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="65" priority="32" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="32" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="64" priority="31" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="31" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="63" priority="29" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="62" priority="30" operator="greaterThan">
+    <cfRule type="top10" dxfId="65" priority="29" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="64" priority="30" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:M37">
-    <cfRule type="top10" dxfId="61" priority="27" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="60" priority="28" operator="greaterThan">
+    <cfRule type="top10" dxfId="63" priority="27" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="62" priority="28" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:M38">
-    <cfRule type="top10" dxfId="59" priority="25" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="58" priority="26" operator="greaterThan">
+    <cfRule type="top10" dxfId="61" priority="25" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="60" priority="26" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:M40">
-    <cfRule type="top10" dxfId="57" priority="23" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="56" priority="24" operator="greaterThan">
+    <cfRule type="top10" dxfId="59" priority="23" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="58" priority="24" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:M41">
-    <cfRule type="top10" dxfId="55" priority="21" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="54" priority="22" operator="greaterThan">
+    <cfRule type="top10" dxfId="57" priority="21" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="56" priority="22" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42:M42">
-    <cfRule type="top10" dxfId="53" priority="19" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="greaterThan">
+    <cfRule type="top10" dxfId="55" priority="19" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="54" priority="20" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:M43">
-    <cfRule type="top10" dxfId="51" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="53" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="52" priority="18" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:M44">
-    <cfRule type="top10" dxfId="49" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="48" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="51" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55:O55">
-    <cfRule type="top10" dxfId="47" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="49" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="48" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:R55">
-    <cfRule type="top10" dxfId="45" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="44" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="47" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:M56">
-    <cfRule type="top10" dxfId="43" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="42" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="45" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56:P56">
-    <cfRule type="top10" dxfId="41" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="43" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:S56">
-    <cfRule type="top10" dxfId="39" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="41" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T56:V56">
-    <cfRule type="top10" dxfId="37" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="39" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56:Y56">
-    <cfRule type="top10" dxfId="35" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="37" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16766,14 +17047,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="33" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="35" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="32" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="34" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="31" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="33" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17113,62 +17394,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="top10" dxfId="29" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="top10" dxfId="28" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="top10" dxfId="27" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="29" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="top10" dxfId="25" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="27" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="top10" dxfId="23" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="25" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="top10" dxfId="21" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="23" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="top10" dxfId="19" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="21" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="top10" dxfId="17" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="19" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="top10" dxfId="15" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="17" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="15" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:E17">
-    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="13" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17504,20 +17785,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="9" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="11" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="8" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="10" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="9" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="5" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
log and prep for new experiment
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -2072,7 +2072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="234">
   <si>
     <t>Test Group</t>
   </si>
@@ -2771,6 +2771,9 @@
   </si>
   <si>
     <t>12gX.0.2</t>
+  </si>
+  <si>
+    <t>09.02.txt</t>
   </si>
 </sst>
 </file>
@@ -13407,13 +13410,16 @@
       </c>
       <c r="F112" s="3">
         <f t="shared" si="47"/>
-        <v>0.60606061408816669</v>
+        <v>1.0437710578192749</v>
       </c>
       <c r="G112" s="5">
         <v>42572</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>217</v>
       </c>
@@ -13432,35 +13438,44 @@
       </c>
       <c r="F113" s="3">
         <f t="shared" si="47"/>
-        <v>0.60606061408816669</v>
+        <v>1.0437710578192749</v>
       </c>
       <c r="G113" s="5">
         <v>42572</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>218</v>
       </c>
       <c r="B114" t="s">
         <v>212</v>
       </c>
+      <c r="C114" s="1">
+        <v>0.43333333929379703</v>
+      </c>
       <c r="D114" s="1">
         <v>0.33</v>
       </c>
       <c r="E114" s="3">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>1.3131313311933244</v>
       </c>
       <c r="F114" s="3">
         <f t="shared" si="47"/>
-        <v>0.60606061408816669</v>
+        <v>1.0437710578192749</v>
       </c>
       <c r="G114" s="5">
         <v>42572</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>224</v>
       </c>
@@ -13482,7 +13497,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -13504,7 +13519,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>226</v>
       </c>
@@ -13526,7 +13541,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -13548,7 +13563,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>228</v>
       </c>
@@ -13570,7 +13585,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -13592,7 +13607,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>230</v>
       </c>
@@ -13614,7 +13629,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>231</v>
       </c>
@@ -13636,7 +13651,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
Log and prep for next experiment
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -2072,7 +2072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="235">
   <si>
     <t>Test Group</t>
   </si>
@@ -2774,6 +2774,9 @@
   </si>
   <si>
     <t>09.02.txt</t>
+  </si>
+  <si>
+    <t>09.41.txt</t>
   </si>
 </sst>
 </file>
@@ -10196,8 +10199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13482,19 +13485,25 @@
       <c r="B115" t="s">
         <v>221</v>
       </c>
+      <c r="C115" s="1">
+        <v>0.266666669646898</v>
+      </c>
       <c r="D115" s="1">
         <v>0.33</v>
       </c>
       <c r="E115" s="3">
         <f t="shared" ref="E115:E123" si="48">C115/D115</f>
-        <v>0</v>
+        <v>0.80808081711181212</v>
       </c>
       <c r="F115" s="3">
         <f t="shared" ref="F115:F123" si="49">AVERAGEIF(B:B,B115,E:E)</f>
-        <v>0</v>
+        <v>1.1111111301765677</v>
       </c>
       <c r="G115" s="5">
         <v>42572</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -13504,19 +13513,25 @@
       <c r="B116" t="s">
         <v>221</v>
       </c>
+      <c r="C116" s="1">
+        <v>0.26666667064030902</v>
+      </c>
       <c r="D116" s="1">
         <v>0.33</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>0.80808082012214855</v>
       </c>
       <c r="F116" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.1111111301765677</v>
       </c>
       <c r="G116" s="5">
         <v>42572</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -13526,19 +13541,25 @@
       <c r="B117" t="s">
         <v>221</v>
       </c>
+      <c r="C117" s="1">
+        <v>0.56666667858759501</v>
+      </c>
       <c r="D117" s="1">
         <v>0.33</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.7171717532957425</v>
       </c>
       <c r="F117" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.1111111301765677</v>
       </c>
       <c r="G117" s="5">
         <v>42572</v>
+      </c>
+      <c r="H117" s="5" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating dataset so I don't have that nonsense with the too-short song
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -964,6 +964,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="B124" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">20g.start0: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>originally was 120g.start, but threw out these results from that group because I changed the dataset.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2072,7 +2093,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="239">
   <si>
     <t>Test Group</t>
   </si>
@@ -2777,6 +2798,18 @@
   </si>
   <si>
     <t>09.41.txt</t>
+  </si>
+  <si>
+    <t>120g.start0</t>
+  </si>
+  <si>
+    <t>12gS0.0.0</t>
+  </si>
+  <si>
+    <t>12gS0.0.1</t>
+  </si>
+  <si>
+    <t>12gS0.0.2</t>
   </si>
 </sst>
 </file>
@@ -2890,47 +2923,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3758,6 +3751,86 @@
           <color rgb="FF00B050"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -10197,10 +10270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13485,25 +13558,19 @@
       <c r="B115" t="s">
         <v>221</v>
       </c>
-      <c r="C115" s="1">
-        <v>0.266666669646898</v>
-      </c>
       <c r="D115" s="1">
         <v>0.33</v>
       </c>
       <c r="E115" s="3">
-        <f t="shared" ref="E115:E123" si="48">C115/D115</f>
-        <v>0.80808081711181212</v>
+        <f t="shared" ref="E115:E126" si="48">C115/D115</f>
+        <v>0</v>
       </c>
       <c r="F115" s="3">
-        <f t="shared" ref="F115:F123" si="49">AVERAGEIF(B:B,B115,E:E)</f>
-        <v>1.1111111301765677</v>
+        <f t="shared" ref="F115:F126" si="49">AVERAGEIF(B:B,B115,E:E)</f>
+        <v>0</v>
       </c>
       <c r="G115" s="5">
         <v>42572</v>
-      </c>
-      <c r="H115" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -13513,25 +13580,19 @@
       <c r="B116" t="s">
         <v>221</v>
       </c>
-      <c r="C116" s="1">
-        <v>0.26666667064030902</v>
-      </c>
       <c r="D116" s="1">
         <v>0.33</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="48"/>
-        <v>0.80808082012214855</v>
+        <v>0</v>
       </c>
       <c r="F116" s="3">
         <f t="shared" si="49"/>
-        <v>1.1111111301765677</v>
+        <v>0</v>
       </c>
       <c r="G116" s="5">
         <v>42572</v>
-      </c>
-      <c r="H116" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -13541,25 +13602,19 @@
       <c r="B117" t="s">
         <v>221</v>
       </c>
-      <c r="C117" s="1">
-        <v>0.56666667858759501</v>
-      </c>
       <c r="D117" s="1">
         <v>0.33</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="48"/>
-        <v>1.7171717532957425</v>
+        <v>0</v>
       </c>
       <c r="F117" s="3">
         <f t="shared" si="49"/>
-        <v>1.1111111301765677</v>
+        <v>0</v>
       </c>
       <c r="G117" s="5">
         <v>42572</v>
-      </c>
-      <c r="H117" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -13694,16 +13749,100 @@
         <v>42572</v>
       </c>
     </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>236</v>
+      </c>
+      <c r="B124" t="s">
+        <v>235</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0.266666669646898</v>
+      </c>
+      <c r="D124" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E124" s="3">
+        <f t="shared" si="48"/>
+        <v>0.80808081711181212</v>
+      </c>
+      <c r="F124" s="3">
+        <f t="shared" si="49"/>
+        <v>1.1111111301765677</v>
+      </c>
+      <c r="G124" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>237</v>
+      </c>
+      <c r="B125" t="s">
+        <v>235</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.26666667064030902</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E125" s="3">
+        <f t="shared" si="48"/>
+        <v>0.80808082012214855</v>
+      </c>
+      <c r="F125" s="3">
+        <f t="shared" si="49"/>
+        <v>1.1111111301765677</v>
+      </c>
+      <c r="G125" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>238</v>
+      </c>
+      <c r="B126" t="s">
+        <v>235</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0.56666667858759501</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E126" s="3">
+        <f t="shared" si="48"/>
+        <v>1.7171717532957425</v>
+      </c>
+      <c r="F126" s="3">
+        <f t="shared" si="49"/>
+        <v>1.1111111301765677</v>
+      </c>
+      <c r="G126" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="71" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="67" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="70" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="69" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="68" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C1:C114 C118:C1048576">
+    <cfRule type="top10" dxfId="65" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14913,98 +15052,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="67" priority="32" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="63" priority="32" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="66" priority="31" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="62" priority="31" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="65" priority="29" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="64" priority="30" operator="greaterThan">
+    <cfRule type="top10" dxfId="61" priority="29" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="60" priority="30" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:M37">
-    <cfRule type="top10" dxfId="63" priority="27" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="62" priority="28" operator="greaterThan">
+    <cfRule type="top10" dxfId="59" priority="27" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="58" priority="28" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:M38">
-    <cfRule type="top10" dxfId="61" priority="25" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="60" priority="26" operator="greaterThan">
+    <cfRule type="top10" dxfId="57" priority="25" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="56" priority="26" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:M40">
-    <cfRule type="top10" dxfId="59" priority="23" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="58" priority="24" operator="greaterThan">
+    <cfRule type="top10" dxfId="55" priority="23" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="54" priority="24" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:M41">
-    <cfRule type="top10" dxfId="57" priority="21" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="56" priority="22" operator="greaterThan">
+    <cfRule type="top10" dxfId="53" priority="21" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="52" priority="22" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42:M42">
-    <cfRule type="top10" dxfId="55" priority="19" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="54" priority="20" operator="greaterThan">
+    <cfRule type="top10" dxfId="51" priority="19" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="50" priority="20" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:M43">
-    <cfRule type="top10" dxfId="53" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="52" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="49" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="48" priority="18" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:M44">
-    <cfRule type="top10" dxfId="51" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="50" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="47" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="46" priority="16" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55:O55">
-    <cfRule type="top10" dxfId="49" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="48" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="45" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:R55">
-    <cfRule type="top10" dxfId="47" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="46" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="43" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:M56">
-    <cfRule type="top10" dxfId="45" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="41" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56:P56">
-    <cfRule type="top10" dxfId="43" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="39" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:S56">
-    <cfRule type="top10" dxfId="41" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="37" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T56:V56">
-    <cfRule type="top10" dxfId="39" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="35" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56:Y56">
-    <cfRule type="top10" dxfId="37" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="33" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17083,14 +17222,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="35" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="31" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="34" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="30" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="33" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="29" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17430,62 +17569,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="top10" dxfId="31" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="27" priority="20" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="top10" dxfId="30" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="26" priority="19" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="top10" dxfId="29" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="25" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="top10" dxfId="27" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="23" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="top10" dxfId="25" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="21" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="top10" dxfId="23" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="19" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="top10" dxfId="21" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="17" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="top10" dxfId="19" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="15" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="top10" dxfId="17" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="13" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="top10" dxfId="15" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="11" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:E17">
-    <cfRule type="top10" dxfId="13" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="9" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17821,20 +17960,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="11" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="7" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="10" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="6" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="9" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="5" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="7" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Prep for final run in this series
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -2093,7 +2093,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="240">
   <si>
     <t>Test Group</t>
   </si>
@@ -2810,6 +2810,9 @@
   </si>
   <si>
     <t>12gS0.0.2</t>
+  </si>
+  <si>
+    <t>10.02.txt</t>
   </si>
 </sst>
 </file>
@@ -2923,7 +2926,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="76">
+  <dxfs count="74">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3751,26 +3754,6 @@
           <color rgb="FF00B050"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -10273,7 +10256,7 @@
   <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+      <selection activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13558,19 +13541,25 @@
       <c r="B115" t="s">
         <v>221</v>
       </c>
+      <c r="C115" s="1">
+        <v>0.46666666666666601</v>
+      </c>
       <c r="D115" s="1">
         <v>0.33</v>
       </c>
       <c r="E115" s="3">
         <f t="shared" ref="E115:E126" si="48">C115/D115</f>
-        <v>0</v>
+        <v>1.4141414141414121</v>
       </c>
       <c r="F115" s="3">
         <f t="shared" ref="F115:F126" si="49">AVERAGEIF(B:B,B115,E:E)</f>
-        <v>0</v>
+        <v>1.0101010156199575</v>
       </c>
       <c r="G115" s="5">
         <v>42572</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -13580,19 +13569,25 @@
       <c r="B116" t="s">
         <v>221</v>
       </c>
+      <c r="C116" s="1">
+        <v>0.33333333730697601</v>
+      </c>
       <c r="D116" s="1">
         <v>0.33</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.0101010221423514</v>
       </c>
       <c r="F116" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0101010156199575</v>
       </c>
       <c r="G116" s="5">
         <v>42572</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -13602,19 +13597,25 @@
       <c r="B117" t="s">
         <v>221</v>
       </c>
+      <c r="C117" s="1">
+        <v>0.20000000149011599</v>
+      </c>
       <c r="D117" s="1">
         <v>0.33</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>0.60606061057610905</v>
       </c>
       <c r="F117" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0101010156199575</v>
       </c>
       <c r="G117" s="5">
         <v>42572</v>
+      </c>
+      <c r="H117" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -13624,19 +13625,25 @@
       <c r="B118" t="s">
         <v>222</v>
       </c>
+      <c r="C118" s="1">
+        <v>0.36666666766007699</v>
+      </c>
       <c r="D118" s="1">
         <v>0.33</v>
       </c>
       <c r="E118" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.1111111141214454</v>
       </c>
       <c r="F118" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0101010201354603</v>
       </c>
       <c r="G118" s="5">
         <v>42572</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -13646,19 +13653,25 @@
       <c r="B119" t="s">
         <v>222</v>
       </c>
+      <c r="C119" s="1">
+        <v>0.300000005960464</v>
+      </c>
       <c r="D119" s="1">
         <v>0.33</v>
       </c>
       <c r="E119" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>0.90909092715292117</v>
       </c>
       <c r="F119" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0101010201354603</v>
       </c>
       <c r="G119" s="5">
         <v>42572</v>
+      </c>
+      <c r="H119" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -13668,19 +13681,25 @@
       <c r="B120" t="s">
         <v>222</v>
       </c>
+      <c r="C120" s="1">
+        <v>0.33333333631356499</v>
+      </c>
       <c r="D120" s="1">
         <v>0.33</v>
       </c>
       <c r="E120" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.010101019132015</v>
       </c>
       <c r="F120" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0101010201354603</v>
       </c>
       <c r="G120" s="5">
         <v>42572</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Prep for verify, but also do a bit of multi-training
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -2093,7 +2093,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="241">
   <si>
     <t>Test Group</t>
   </si>
@@ -2813,6 +2813,9 @@
   </si>
   <si>
     <t>10.02.txt</t>
+  </si>
+  <si>
+    <t>10.26.txt</t>
   </si>
 </sst>
 </file>
@@ -10256,7 +10259,7 @@
   <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="H120" sqref="H120"/>
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13709,19 +13712,25 @@
       <c r="B121" t="s">
         <v>223</v>
       </c>
+      <c r="C121" s="1">
+        <v>0.46666666666666601</v>
+      </c>
       <c r="D121" s="1">
         <v>0.33</v>
       </c>
       <c r="E121" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.4141414141414121</v>
       </c>
       <c r="F121" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0437710477848232</v>
       </c>
       <c r="G121" s="5">
         <v>42572</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -13731,19 +13740,25 @@
       <c r="B122" t="s">
         <v>223</v>
       </c>
+      <c r="C122" s="1">
+        <v>0.333333334326744</v>
+      </c>
       <c r="D122" s="1">
         <v>0.33</v>
       </c>
       <c r="E122" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1.0101010131113455</v>
       </c>
       <c r="F122" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0437710477848232</v>
       </c>
       <c r="G122" s="5">
         <v>42572</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -13753,19 +13768,25 @@
       <c r="B123" t="s">
         <v>223</v>
       </c>
+      <c r="C123" s="1">
+        <v>0.23333333631356501</v>
+      </c>
       <c r="D123" s="1">
         <v>0.33</v>
       </c>
       <c r="E123" s="3">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>0.70707071610171213</v>
       </c>
       <c r="F123" s="3">
         <f t="shared" si="49"/>
-        <v>0</v>
+        <v>1.0437710477848232</v>
       </c>
       <c r="G123" s="5">
         <v>42572</v>
+      </c>
+      <c r="H123" s="5" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
And build ourselves some new graphs
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24580" windowHeight="15540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -1989,6 +1989,49 @@
         </r>
       </text>
     </comment>
+    <comment ref="B22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">120.start, 120.minute, 120.mix: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Rerunning the 15.comparison series, using a new The120 dataset to prevent overfitting.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">120g.start, 120g.minute, 120g.mix: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>The same test as above, but using a generator feed rather than a cache, which allows for more mixing throughout, when applicable.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2093,7 +2136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="246">
   <si>
     <t>Test Group</t>
   </si>
@@ -2944,47 +2987,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="74">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="138">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3048,26 +3051,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FF00B050"/>
@@ -3302,72 +3285,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF00B050"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF00B050"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF00B050"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF00B050"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FF00B050"/>
@@ -3758,6 +3675,22 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -3766,6 +3699,152 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3844,6 +3923,814 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF00B050"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF00B050"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF00B050"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF00B050"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -3857,8 +4744,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF729FCF"/>
       <color rgb="FFFCAF3E"/>
-      <color rgb="FF729FCF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -5863,6 +6750,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7128,6 +8016,1033 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
+              <a:t>Accuracy of Tests at Varying</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000" baseline="0">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
+              <a:t> Sample Locations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="4000">
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$42:$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$C$42:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.266666667660077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51724139164234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.233333339293797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$D$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$42:$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$D$42:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.300000002980232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20000000099341</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.366666668653488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$E$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$42:$B$44</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$E$42:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.333333339293797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.250000002128737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.433333339293797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2132016512"/>
+        <c:axId val="-2068115872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2132016512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2068115872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2068115872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2132016512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
+              <a:t>Accuracy of Tests at Varying</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000" baseline="0">
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:rPr>
+              <a:t> Sample Locations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="4000">
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Avenir Book" charset="0"/>
+              <a:ea typeface="Avenir Book" charset="0"/>
+              <a:cs typeface="Avenir Book" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$C$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$C$47:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.466666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.366666667660077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.466666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$D$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$D$47:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.333333337306976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.300000005960464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333333334326744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$E$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15.comparison'!$E$47:$E$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.200000001490116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.333333336313565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.233333336313565</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2067540256"/>
+        <c:axId val="-2067538464"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2067540256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2067538464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2067538464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avenir Book" charset="0"/>
+                <a:ea typeface="Avenir Book" charset="0"/>
+                <a:cs typeface="Avenir Book" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2067540256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7289,6 +9204,86 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9843,6 +11838,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9977,16 +12978,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>218130</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>421330</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>703735</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>81435</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10000,6 +13001,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>485605</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>498305</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10273,8 +13338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13974,14 +17039,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="69" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="137" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="68" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="136" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C114 C118:C1048576">
-    <cfRule type="top10" dxfId="67" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="66" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="135" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="134" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15191,98 +18256,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="65" priority="32" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="133" priority="32" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="64" priority="31" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="132" priority="31" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="top10" dxfId="63" priority="29" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="62" priority="30" operator="greaterThan">
+    <cfRule type="top10" dxfId="131" priority="29" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="130" priority="30" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:M37">
-    <cfRule type="top10" dxfId="61" priority="27" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="60" priority="28" operator="greaterThan">
+    <cfRule type="top10" dxfId="129" priority="27" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="128" priority="28" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:M38">
-    <cfRule type="top10" dxfId="59" priority="25" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="58" priority="26" operator="greaterThan">
+    <cfRule type="top10" dxfId="127" priority="25" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="126" priority="26" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:M40">
-    <cfRule type="top10" dxfId="57" priority="23" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="56" priority="24" operator="greaterThan">
+    <cfRule type="top10" dxfId="125" priority="23" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="124" priority="24" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:M41">
-    <cfRule type="top10" dxfId="55" priority="21" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="54" priority="22" operator="greaterThan">
+    <cfRule type="top10" dxfId="123" priority="21" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="122" priority="22" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42:M42">
-    <cfRule type="top10" dxfId="53" priority="19" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="greaterThan">
+    <cfRule type="top10" dxfId="121" priority="19" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="120" priority="20" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:M43">
-    <cfRule type="top10" dxfId="51" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="119" priority="17" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="118" priority="18" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:M44">
-    <cfRule type="top10" dxfId="49" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="48" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="117" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="116" priority="16" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55:O55">
-    <cfRule type="top10" dxfId="47" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="115" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="114" priority="14" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:R55">
-    <cfRule type="top10" dxfId="45" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="44" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="113" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="112" priority="12" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K56:M56">
-    <cfRule type="top10" dxfId="43" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="42" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="111" priority="9" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="110" priority="10" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56:P56">
-    <cfRule type="top10" dxfId="41" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="109" priority="7" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="108" priority="8" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q56:S56">
-    <cfRule type="top10" dxfId="39" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="107" priority="5" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="106" priority="6" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T56:V56">
-    <cfRule type="top10" dxfId="37" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="105" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="104" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W56:Y56">
-    <cfRule type="top10" dxfId="35" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="103" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17361,14 +20426,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E71">
-    <cfRule type="top10" dxfId="33" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="101" priority="4" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F71">
-    <cfRule type="top10" dxfId="32" priority="3" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="100" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C71">
-    <cfRule type="top10" dxfId="31" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="99" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="98" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17380,10 +20445,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="41" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
+      <selection activeCell="AC86" sqref="AC86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17702,68 +20767,720 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.26666666766007702</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" ref="E22:E39" si="3">C22/D22</f>
+        <v>0.80808081109114249</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" ref="F22:F39" si="4">AVERAGEIF(B:B,B22,E:E)</f>
+        <v>0.90909091912535944</v>
+      </c>
+      <c r="G22" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>209</v>
+      </c>
+      <c r="B23" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.30000000298023199</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="3"/>
+        <v>0.90909091812191511</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.90909091912535944</v>
+      </c>
+      <c r="G23" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.33333333929379699</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0101010281630212</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.90909091912535944</v>
+      </c>
+      <c r="G24" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.51724139164233995</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5673981564919393</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97701150986311802</v>
+      </c>
+      <c r="G25" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.20000000099341</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="3"/>
+        <v>0.60606060907093939</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97701150986311802</v>
+      </c>
+      <c r="G26" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>215</v>
+      </c>
+      <c r="B27" t="s">
+        <v>211</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.25000000212873702</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="3"/>
+        <v>0.75757576402647575</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97701150986311802</v>
+      </c>
+      <c r="G27" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B28" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.23333333929379699</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="3"/>
+        <v>0.70707072513271807</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710578192749</v>
+      </c>
+      <c r="G28" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.36666666865348801</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1111111171317818</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710578192749</v>
+      </c>
+      <c r="G29" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" t="s">
+        <v>212</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.43333333929379703</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3131313311933244</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710578192749</v>
+      </c>
+      <c r="G30" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4141414141414121</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010156199575</v>
+      </c>
+      <c r="G31" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.33333333730697601</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0101010221423514</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010156199575</v>
+      </c>
+      <c r="G32" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" t="s">
+        <v>221</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.20000000149011599</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>0.60606061057610905</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010156199575</v>
+      </c>
+      <c r="G33" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.36666666766007699</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1111111141214454</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010201354603</v>
+      </c>
+      <c r="G34" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.300000005960464</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
+        <v>0.90909092715292117</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010201354603</v>
+      </c>
+      <c r="G35" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B36" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.33333333631356499</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="3"/>
+        <v>1.010101019132015</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0101010201354603</v>
+      </c>
+      <c r="G36" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B37" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E37" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4141414141414121</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710477848232</v>
+      </c>
+      <c r="G37" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.333333334326744</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0101010131113455</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710477848232</v>
+      </c>
+      <c r="G38" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.23333333631356501</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="3"/>
+        <v>0.70707071610171213</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0437710477848232</v>
+      </c>
+      <c r="G39" s="5">
+        <v>42572</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41" t="s">
+        <v>202</v>
+      </c>
+      <c r="E41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>199</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.26666666766007702</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.30000000298023199</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.33333333929379699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>200</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.51724139164233995</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.20000000099341</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.25000000212873702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.23333333929379699</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.36666666865348801</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.43333333929379703</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.33333333730697601</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.20000000149011599</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>200</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.36666666766007699</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.300000005960464</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.33333333631356499</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>206</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.333333334326744</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.23333333631356501</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E9">
-    <cfRule type="top10" dxfId="29" priority="20" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="97" priority="56" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F9">
-    <cfRule type="top10" dxfId="28" priority="19" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="96" priority="55" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C9">
-    <cfRule type="top10" dxfId="27" priority="17" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="greaterThan">
+    <cfRule type="top10" dxfId="95" priority="53" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="94" priority="54" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="top10" dxfId="25" priority="15" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="greaterThan">
+    <cfRule type="top10" dxfId="93" priority="51" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="92" priority="52" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="top10" dxfId="23" priority="13" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
+    <cfRule type="top10" dxfId="91" priority="49" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="90" priority="50" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="top10" dxfId="21" priority="11" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+    <cfRule type="top10" dxfId="89" priority="47" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="88" priority="48" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="top10" dxfId="19" priority="9" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
+    <cfRule type="top10" dxfId="87" priority="45" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="86" priority="46" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="top10" dxfId="17" priority="7" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="top10" dxfId="85" priority="43" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="84" priority="44" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="top10" dxfId="15" priority="5" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
+    <cfRule type="top10" dxfId="83" priority="41" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="top10" dxfId="13" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="81" priority="39" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="80" priority="40" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:E17">
-    <cfRule type="top10" dxfId="11" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="79" priority="37" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="78" priority="38" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:E39">
+    <cfRule type="top10" dxfId="71" priority="36" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22:F39">
+    <cfRule type="top10" dxfId="69" priority="35" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C30 C34:C39">
+    <cfRule type="top10" dxfId="67" priority="33" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="66" priority="34" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:E42">
+    <cfRule type="top10" dxfId="31" priority="15" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:E43">
+    <cfRule type="top10" dxfId="27" priority="13" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:E44">
+    <cfRule type="top10" dxfId="23" priority="11" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:E48">
+    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:E49">
+    <cfRule type="top10" dxfId="3" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18099,20 +21816,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="9" priority="6" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="77" priority="6" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="top10" dxfId="8" priority="5" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="5" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C10:C1048576">
-    <cfRule type="top10" dxfId="7" priority="3" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="top10" dxfId="75" priority="3" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="top10" dxfId="5" priority="1" percent="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="top10" dxfId="73" priority="1" percent="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="greaterThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Remove incorrect 'guess' lines from charts
</commit_message>
<xml_diff>
--- a/logs/Experiment Log.xlsx
+++ b/logs/Experiment Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greypatterson/Documents/More/Bitbucket/nAud/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4309,11 +4309,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2133470624"/>
-        <c:axId val="-2133474112"/>
+        <c:axId val="-2147032272"/>
+        <c:axId val="-2147028784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133470624"/>
+        <c:axId val="-2147032272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4356,7 +4356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133474112"/>
+        <c:crossAx val="-2147028784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4364,7 +4364,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133474112"/>
+        <c:axId val="-2147028784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4416,7 +4416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133470624"/>
+        <c:crossAx val="-2147032272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4827,11 +4827,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2133602448"/>
-        <c:axId val="-2133605952"/>
+        <c:axId val="2143231536"/>
+        <c:axId val="2143235024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133602448"/>
+        <c:axId val="2143231536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4874,7 +4874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133605952"/>
+        <c:crossAx val="2143235024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4882,7 +4882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133605952"/>
+        <c:axId val="2143235024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -4933,7 +4933,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133602448"/>
+        <c:crossAx val="2143231536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5849,11 +5849,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2133728224"/>
-        <c:axId val="-2133731664"/>
+        <c:axId val="-2146792576"/>
+        <c:axId val="-2146789152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133728224"/>
+        <c:axId val="-2146792576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5896,7 +5896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133731664"/>
+        <c:crossAx val="-2146789152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5904,7 +5904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133731664"/>
+        <c:axId val="-2146789152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5943,7 +5943,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133728224"/>
+        <c:crossAx val="-2146792576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6008,6 +6008,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6516,11 +6517,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2133793808"/>
-        <c:axId val="-2133797504"/>
+        <c:axId val="-2146369056"/>
+        <c:axId val="-2146365376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133793808"/>
+        <c:axId val="-2146369056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6563,7 +6564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133797504"/>
+        <c:crossAx val="-2146365376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6571,7 +6572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133797504"/>
+        <c:axId val="-2146365376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6622,7 +6623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133793808"/>
+        <c:crossAx val="-2146369056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7128,11 +7129,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2131455760"/>
-        <c:axId val="-2131458080"/>
+        <c:axId val="-2146299360"/>
+        <c:axId val="-2146295680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131455760"/>
+        <c:axId val="-2146299360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7175,7 +7176,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131458080"/>
+        <c:crossAx val="-2146295680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7183,7 +7184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131458080"/>
+        <c:axId val="-2146295680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7220,7 +7221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131455760"/>
+        <c:crossAx val="-2146299360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7552,11 +7553,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2131493664"/>
-        <c:axId val="-2131497168"/>
+        <c:axId val="2088633392"/>
+        <c:axId val="2088642000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131493664"/>
+        <c:axId val="2088633392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7599,7 +7600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131497168"/>
+        <c:crossAx val="2088642000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7607,7 +7608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131497168"/>
+        <c:axId val="2088642000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7644,7 +7645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131493664"/>
+        <c:crossAx val="2088633392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7931,131 +7932,12 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="Avenir Book" charset="0"/>
-                    <a:ea typeface="Avenir Book" charset="0"/>
-                    <a:cs typeface="Avenir Book" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="1"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'15.comparison'!$B$47:$B$49</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Start</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1 Minute</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Random Points</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'15.comparison'!$D$47:$D$49</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.333333337306976</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.300000005960464</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.333333334326744</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'15.comparison'!$E$46</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Test 3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="729FCF"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
             <c:dLbl>
-              <c:idx val="2"/>
+              <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.0"/>
-                  <c:y val="-0.0235849056603774"/>
+                  <c:y val="0.00485262414884845"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="outEnd"/>
@@ -8148,6 +8030,146 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>'15.comparison'!$D$47:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.333333337306976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.300000005960464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333333334326744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'15.comparison'!$E$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="729FCF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.000919857055662009"/>
+                  <c:y val="-0.0025568616742292"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Avenir Book" charset="0"/>
+                    <a:ea typeface="Avenir Book" charset="0"/>
+                    <a:cs typeface="Avenir Book" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15.comparison'!$B$47:$B$49</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Start</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1 Minute</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Random Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>'15.comparison'!$E$47:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
@@ -8175,11 +8197,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2131553344"/>
-        <c:axId val="-2131556912"/>
+        <c:axId val="-2146916272"/>
+        <c:axId val="-2146864176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2131553344"/>
+        <c:axId val="-2146916272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8222,7 +8244,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131556912"/>
+        <c:crossAx val="-2146864176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8230,7 +8252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131556912"/>
+        <c:axId val="-2146864176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8269,7 +8291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131553344"/>
+        <c:crossAx val="-2146916272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12402,13 +12424,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>115711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>498305</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>64911</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12436,12 +12458,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.12643</cdr:x>
-      <cdr:y>0.51782</cdr:y>
+      <cdr:x>0.12541</cdr:x>
+      <cdr:y>0.4028</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.93421</cdr:x>
-      <cdr:y>0.51782</cdr:y>
+      <cdr:x>0.93319</cdr:x>
+      <cdr:y>0.4028</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -12450,8 +12472,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1712985" y="4357901"/>
-          <a:ext cx="10944077" cy="0"/>
+          <a:off x="1731444" y="3162516"/>
+          <a:ext cx="11152609" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -12476,11 +12498,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.92159</cdr:x>
-      <cdr:y>0.49191</cdr:y>
+      <cdr:y>0.37688</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.99693</cdr:x>
-      <cdr:y>0.54223</cdr:y>
+      <cdr:y>0.4272</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -12489,8 +12511,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="12723950" y="3862220"/>
-          <a:ext cx="1040210" cy="395040"/>
+          <a:off x="12723926" y="2959082"/>
+          <a:ext cx="1040181" cy="395084"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -12781,8 +12803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:H123"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17804,9 +17826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:H28"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19890,8 +19912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K91" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="AC91" sqref="AC91"/>
+    <sheetView tabSelected="1" topLeftCell="J90" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="AB100" sqref="AB100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>